<commit_message>
add a new model for pattern 3 and modify corresponding docx
</commit_message>
<xml_diff>
--- a/processing_directory/results/spl_cation_data.xlsx
+++ b/processing_directory/results/spl_cation_data.xlsx
@@ -478,28 +478,28 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.001954131951018266</v>
+        <v>0.001302754634012177</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0005880428724123483</v>
+        <v>0.0003920285816082322</v>
       </c>
       <c r="C2" t="n">
-        <v>2.633807742541642</v>
+        <v>1.755871828361095</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2855126138129474</v>
+        <v>0.1903417425419649</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4157498467139212</v>
+        <v>0.2771665644759475</v>
       </c>
       <c r="F2" t="n">
-        <v>0.004303343615234352</v>
+        <v>0.002868895743489568</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01257538799475505</v>
+        <v>0.008383591996503363</v>
       </c>
       <c r="H2" t="n">
-        <v>1.183306537497344</v>
+        <v>0.7888710249982297</v>
       </c>
     </row>
     <row r="3">
@@ -507,51 +507,51 @@
         <v>1e-07</v>
       </c>
       <c r="B3" t="n">
-        <v>0.003579211400793524</v>
+        <v>0.00238614093386235</v>
       </c>
       <c r="C3" t="n">
-        <v>2.666704544013781</v>
+        <v>1.777803029342521</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2767841022015002</v>
+        <v>0.1845227348010002</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3783186404296249</v>
+        <v>0.2522124269530833</v>
       </c>
       <c r="F3" t="n">
-        <v>0.002686456231344947</v>
+        <v>0.001790970820896632</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01275699845250606</v>
+        <v>0.00850466563500404</v>
       </c>
       <c r="H3" t="n">
-        <v>1.183846512762014</v>
+        <v>0.7892310085080095</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.001191387936442807</v>
+        <v>0.0007942586242952042</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0008962895058572986</v>
+        <v>0.000597526337238199</v>
       </c>
       <c r="C4" t="n">
-        <v>2.54242261199706</v>
+        <v>1.69494840799804</v>
       </c>
       <c r="D4" t="n">
-        <v>0.363902322078373</v>
+        <v>0.2426015480522487</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4314219124746943</v>
+        <v>0.2876146083164628</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00336364950050952</v>
+        <v>0.00224243300033968</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01277819336034081</v>
+        <v>0.008518795573560537</v>
       </c>
       <c r="H4" t="n">
-        <v>1.188773488666705</v>
+        <v>0.7925156591111365</v>
       </c>
     </row>
     <row r="5">
@@ -559,25 +559,25 @@
         <v>1e-07</v>
       </c>
       <c r="B5" t="n">
-        <v>0.004446739211868592</v>
+        <v>0.002964492807912395</v>
       </c>
       <c r="C5" t="n">
-        <v>2.570567134250465</v>
+        <v>1.713711422833643</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3442603556899978</v>
+        <v>0.2295069037933319</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3779895651205392</v>
+        <v>0.2519930434136928</v>
       </c>
       <c r="F5" t="n">
-        <v>0.001001279521704851</v>
+        <v>0.0006675196811365674</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01331318904349165</v>
+        <v>0.008875459362327765</v>
       </c>
       <c r="H5" t="n">
-        <v>1.226561252979833</v>
+        <v>0.8177075019865555</v>
       </c>
     </row>
     <row r="6">
@@ -585,77 +585,77 @@
         <v>1e-07</v>
       </c>
       <c r="B6" t="n">
-        <v>0.002986338798565176</v>
+        <v>0.001990892532376784</v>
       </c>
       <c r="C6" t="n">
-        <v>2.637230172337778</v>
+        <v>1.758153448225185</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2943853875770859</v>
+        <v>0.1962569250513906</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3648402636462351</v>
+        <v>0.2432268424308234</v>
       </c>
       <c r="F6" t="n">
-        <v>0.003698413281674564</v>
+        <v>0.00246560885444971</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01021813091190094</v>
+        <v>0.006812087274600626</v>
       </c>
       <c r="H6" t="n">
-        <v>1.217847174690763</v>
+        <v>0.8118981164605087</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.002803298222523445</v>
+        <v>0.001868865481682297</v>
       </c>
       <c r="B7" t="n">
-        <v>0.003916604577993918</v>
+        <v>0.002611069718662612</v>
       </c>
       <c r="C7" t="n">
-        <v>2.314609657039758</v>
+        <v>1.543073104693172</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5974651927348394</v>
+        <v>0.3983101284898929</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3915136226594749</v>
+        <v>0.2610090817729833</v>
       </c>
       <c r="F7" t="n">
-        <v>0.004070345729805549</v>
+        <v>0.002713563819870366</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0109528641077105</v>
+        <v>0.007301909405140333</v>
       </c>
       <c r="H7" t="n">
-        <v>1.211911087240077</v>
+        <v>0.8079407248267182</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.002748268701525228</v>
+        <v>0.001832179134350152</v>
       </c>
       <c r="B8" t="n">
-        <v>0.002953631188232648</v>
+        <v>0.001969087458821765</v>
       </c>
       <c r="C8" t="n">
-        <v>2.588911951619143</v>
+        <v>1.725941301079429</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3200289484745535</v>
+        <v>0.2133526323163691</v>
       </c>
       <c r="E8" t="n">
-        <v>0.395319961078494</v>
+        <v>0.263546640718996</v>
       </c>
       <c r="F8" t="n">
-        <v>0.003990443715097064</v>
+        <v>0.00266029581006471</v>
       </c>
       <c r="G8" t="n">
-        <v>0.01200113356749266</v>
+        <v>0.008000755711661771</v>
       </c>
       <c r="H8" t="n">
-        <v>1.213873311718856</v>
+        <v>0.809248874479237</v>
       </c>
     </row>
     <row r="9">
@@ -663,25 +663,25 @@
         <v>1e-07</v>
       </c>
       <c r="B9" t="n">
-        <v>0.001773027646550057</v>
+        <v>0.001182018431033371</v>
       </c>
       <c r="C9" t="n">
-        <v>2.598947997709922</v>
+        <v>1.732631998473281</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3326044550463793</v>
+        <v>0.2217363033642529</v>
       </c>
       <c r="E9" t="n">
-        <v>0.39616632497266</v>
+        <v>0.2641108833151066</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0009980888181888175</v>
+        <v>0.0006653925454592118</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01327076488702996</v>
+        <v>0.00884717659135331</v>
       </c>
       <c r="H9" t="n">
-        <v>1.188690086894569</v>
+        <v>0.7924600579297125</v>
       </c>
     </row>
     <row r="10">
@@ -689,103 +689,103 @@
         <v>1e-07</v>
       </c>
       <c r="B10" t="n">
-        <v>0.002108641965846138</v>
+        <v>0.001405761310564092</v>
       </c>
       <c r="C10" t="n">
-        <v>2.501632636319646</v>
+        <v>1.667755090879764</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4267455801442451</v>
+        <v>0.2844970534294967</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4336512132039674</v>
+        <v>0.2891008088026449</v>
       </c>
       <c r="F10" t="n">
-        <v>0.003391473935671326</v>
+        <v>0.002260982623780885</v>
       </c>
       <c r="G10" t="n">
-        <v>0.01352809060694333</v>
+        <v>0.00901872707129555</v>
       </c>
       <c r="H10" t="n">
-        <v>1.152644613625889</v>
+        <v>0.7684297424172591</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.002352636201598055</v>
+        <v>0.001568424134398703</v>
       </c>
       <c r="B11" t="n">
-        <v>0.004129777692791217</v>
+        <v>0.002753185128527478</v>
       </c>
       <c r="C11" t="n">
-        <v>2.515809074441534</v>
+        <v>1.677206049627689</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3949502567233697</v>
+        <v>0.2633001711489131</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3941568675708024</v>
+        <v>0.2627712450472016</v>
       </c>
       <c r="F11" t="n">
-        <v>0.003653213062075681</v>
+        <v>0.00243547537471712</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01135490608637733</v>
+        <v>0.00756993739091822</v>
       </c>
       <c r="H11" t="n">
-        <v>1.211731188744611</v>
+        <v>0.8078207924964074</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.001630085310147132</v>
+        <v>0.001086723540098088</v>
       </c>
       <c r="B12" t="n">
-        <v>0.004292136166199154</v>
+        <v>0.002861424110799436</v>
       </c>
       <c r="C12" t="n">
-        <v>2.37216779828552</v>
+        <v>1.581445198857014</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5171241576093007</v>
+        <v>0.3447494384062005</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4904245941807646</v>
+        <v>0.3269497294538431</v>
       </c>
       <c r="F12" t="n">
-        <v>0.003796835828218248</v>
+        <v>0.002531223885478832</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01180131394535065</v>
+        <v>0.00786754263023377</v>
       </c>
       <c r="H12" t="n">
-        <v>1.148194879250741</v>
+        <v>0.7654632528338275</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.001943765314912849</v>
+        <v>0.001295843543275233</v>
       </c>
       <c r="B13" t="n">
-        <v>0.002632154918282547</v>
+        <v>0.001754769945521698</v>
       </c>
       <c r="C13" t="n">
-        <v>2.648242188267645</v>
+        <v>1.76549479217843</v>
       </c>
       <c r="D13" t="n">
-        <v>0.270166904169601</v>
+        <v>0.1801112694464007</v>
       </c>
       <c r="E13" t="n">
-        <v>0.3654275112507137</v>
+        <v>0.2436183408338091</v>
       </c>
       <c r="F13" t="n">
-        <v>0.002634162739690907</v>
+        <v>0.001756108493127272</v>
       </c>
       <c r="G13" t="n">
-        <v>0.01250867577956501</v>
+        <v>0.008339117186376673</v>
       </c>
       <c r="H13" t="n">
-        <v>1.23266417110777</v>
+        <v>0.8217761140718465</v>
       </c>
     </row>
     <row r="14">
@@ -793,181 +793,181 @@
         <v>1e-07</v>
       </c>
       <c r="B14" t="n">
-        <v>0.004789015856716981</v>
+        <v>0.003192677237811321</v>
       </c>
       <c r="C14" t="n">
-        <v>2.517564585089216</v>
+        <v>1.678376390059477</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3806150849650378</v>
+        <v>0.2537433899766918</v>
       </c>
       <c r="E14" t="n">
-        <v>0.4072618239776137</v>
+        <v>0.2715078826517425</v>
       </c>
       <c r="F14" t="n">
-        <v>0.001010953605126825</v>
+        <v>0.0006739690700845498</v>
       </c>
       <c r="G14" t="n">
-        <v>0.01248168755060061</v>
+        <v>0.008321125033733737</v>
       </c>
       <c r="H14" t="n">
-        <v>1.222397998071845</v>
+        <v>0.8149319987145632</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.002335161859660121</v>
+        <v>0.001556774573106747</v>
       </c>
       <c r="B15" t="n">
-        <v>0.004099103529279465</v>
+        <v>0.00273273568618631</v>
       </c>
       <c r="C15" t="n">
-        <v>2.615006766149728</v>
+        <v>1.743337844099819</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2846275394116506</v>
+        <v>0.1897516929411004</v>
       </c>
       <c r="E15" t="n">
-        <v>0.3560771992912217</v>
+        <v>0.2373847995274811</v>
       </c>
       <c r="F15" t="n">
-        <v>0.003955722120020836</v>
+        <v>0.002637148080013891</v>
       </c>
       <c r="G15" t="n">
-        <v>0.01283592337102661</v>
+        <v>0.008557282247351077</v>
       </c>
       <c r="H15" t="n">
-        <v>1.264811166097785</v>
+        <v>0.8432074440651897</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.003539265129040203</v>
+        <v>0.002359510086026802</v>
       </c>
       <c r="B16" t="n">
-        <v>0.002662613995468885</v>
+        <v>0.001775075996979256</v>
       </c>
       <c r="C16" t="n">
-        <v>2.648298054008141</v>
+        <v>1.765532036005427</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2838643231360103</v>
+        <v>0.1892428820906735</v>
       </c>
       <c r="E16" t="n">
-        <v>0.3811668549775656</v>
+        <v>0.2541112366517103</v>
       </c>
       <c r="F16" t="n">
-        <v>0.003663886945426298</v>
+        <v>0.002442591296950865</v>
       </c>
       <c r="G16" t="n">
-        <v>0.01328609638905423</v>
+        <v>0.008857397592702817</v>
       </c>
       <c r="H16" t="n">
-        <v>1.19123583772271</v>
+        <v>0.7941572251484731</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.002712049088676789</v>
+        <v>0.001808032725784526</v>
       </c>
       <c r="B17" t="n">
-        <v>0.003206175598723994</v>
+        <v>0.002137450399149329</v>
       </c>
       <c r="C17" t="n">
-        <v>2.652052709293431</v>
+        <v>1.768035139528954</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2766028838396306</v>
+        <v>0.1844019225597537</v>
       </c>
       <c r="E17" t="n">
-        <v>0.3674291987359381</v>
+        <v>0.2449527991572921</v>
       </c>
       <c r="F17" t="n">
-        <v>0.003281544497128589</v>
+        <v>0.00218769633141906</v>
       </c>
       <c r="G17" t="n">
-        <v>0.01215462694494674</v>
+        <v>0.008103084629964494</v>
       </c>
       <c r="H17" t="n">
-        <v>1.212314790747592</v>
+        <v>0.8082098604983949</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.002356090944873747</v>
+        <v>0.001570727296582498</v>
       </c>
       <c r="B18" t="n">
-        <v>0.002363338337458617</v>
+        <v>0.001575558891639078</v>
       </c>
       <c r="C18" t="n">
-        <v>2.717120616672802</v>
+        <v>1.811413744448534</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2396776552907024</v>
+        <v>0.1597851035271349</v>
       </c>
       <c r="E18" t="n">
-        <v>0.3615673646539149</v>
+        <v>0.2410449097692765</v>
       </c>
       <c r="F18" t="n">
-        <v>0.003991175613314613</v>
+        <v>0.002660783742209742</v>
       </c>
       <c r="G18" t="n">
-        <v>0.01200333472828923</v>
+        <v>0.008002223152192822</v>
       </c>
       <c r="H18" t="n">
-        <v>1.177801858494562</v>
+        <v>0.7852012389963745</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.002750550712197908</v>
+        <v>0.001833700474798605</v>
       </c>
       <c r="B19" t="n">
-        <v>0.004138517208814547</v>
+        <v>0.002759011472543032</v>
       </c>
       <c r="C19" t="n">
-        <v>2.629036092461487</v>
+        <v>1.752690728307658</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2979268679498543</v>
+        <v>0.1986179119665695</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3440562117677851</v>
+        <v>0.2293708078451901</v>
       </c>
       <c r="F19" t="n">
-        <v>0.002662504772902908</v>
+        <v>0.001775003181935272</v>
       </c>
       <c r="G19" t="n">
-        <v>0.01074677247323017</v>
+        <v>0.007164514982153447</v>
       </c>
       <c r="H19" t="n">
-        <v>1.238311934527045</v>
+        <v>0.8255412896846969</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.004427408036937593</v>
+        <v>0.002951605357958396</v>
       </c>
       <c r="B20" t="n">
-        <v>0.004844756564581302</v>
+        <v>0.003229837709720868</v>
       </c>
       <c r="C20" t="n">
-        <v>2.404083278569679</v>
+        <v>1.60272218571312</v>
       </c>
       <c r="D20" t="n">
-        <v>0.525379816535244</v>
+        <v>0.350253211023496</v>
       </c>
       <c r="E20" t="n">
-        <v>0.3847372171855135</v>
+        <v>0.2564914781236757</v>
       </c>
       <c r="F20" t="n">
-        <v>0.004090881518427819</v>
+        <v>0.002727254345618547</v>
       </c>
       <c r="G20" t="n">
-        <v>0.01100812371390988</v>
+        <v>0.00733874914260659</v>
       </c>
       <c r="H20" t="n">
-        <v>1.187424805721726</v>
+        <v>0.7916165371478174</v>
       </c>
     </row>
     <row r="21">
@@ -975,675 +975,675 @@
         <v>1e-07</v>
       </c>
       <c r="B21" t="n">
-        <v>0.002097669907396325</v>
+        <v>0.001398446604930883</v>
       </c>
       <c r="C21" t="n">
-        <v>2.434158159076732</v>
+        <v>1.622772106051154</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5101859055398108</v>
+        <v>0.3401239370265405</v>
       </c>
       <c r="E21" t="n">
-        <v>0.3877556012779624</v>
+        <v>0.2585037341853083</v>
       </c>
       <c r="F21" t="n">
-        <v>0.002699061455403406</v>
+        <v>0.001799374303602271</v>
       </c>
       <c r="G21" t="n">
-        <v>0.01249643465166301</v>
+        <v>0.008330956434442002</v>
       </c>
       <c r="H21" t="n">
-        <v>1.176337465875365</v>
+        <v>0.7842249772502433</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.00124723040555743</v>
+        <v>0.0008314869370382868</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0006255334581865823</v>
+        <v>0.0004170223054577215</v>
       </c>
       <c r="C22" t="n">
-        <v>2.1769967759781</v>
+        <v>1.451331183985401</v>
       </c>
       <c r="D22" t="n">
-        <v>0.7313493801834924</v>
+        <v>0.4875662534556617</v>
       </c>
       <c r="E22" t="n">
-        <v>0.515617550200851</v>
+        <v>0.343745033467234</v>
       </c>
       <c r="F22" t="n">
-        <v>0.005281964592321855</v>
+        <v>0.00352130972821457</v>
       </c>
       <c r="G22" t="n">
-        <v>0.009029562739168369</v>
+        <v>0.006019708492778914</v>
       </c>
       <c r="H22" t="n">
-        <v>1.103806160497781</v>
+        <v>0.7358707736651874</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.002151981628018963</v>
+        <v>0.001434654418679309</v>
       </c>
       <c r="B23" t="n">
-        <v>0.001295160705252748</v>
+        <v>0.0008634404701684985</v>
       </c>
       <c r="C23" t="n">
-        <v>1.851980568199051</v>
+        <v>1.234653712132701</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9956628981550681</v>
+        <v>0.6637752654367121</v>
       </c>
       <c r="E23" t="n">
-        <v>0.6367331969390065</v>
+        <v>0.4244887979593377</v>
       </c>
       <c r="F23" t="n">
-        <v>0.008019919837145057</v>
+        <v>0.005346613224763371</v>
       </c>
       <c r="G23" t="n">
-        <v>0.007962948587784657</v>
+        <v>0.005308632391856438</v>
       </c>
       <c r="H23" t="n">
-        <v>1.068924450438342</v>
+        <v>0.7126163002922283</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.002761981119780534</v>
+        <v>0.001841320746520356</v>
       </c>
       <c r="B24" t="n">
-        <v>0.005046226037753272</v>
+        <v>0.003364150691835514</v>
       </c>
       <c r="C24" t="n">
-        <v>2.431629172117636</v>
+        <v>1.621086114745091</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4691804949721734</v>
+        <v>0.3127869966481155</v>
       </c>
       <c r="E24" t="n">
-        <v>0.3890429732669063</v>
+        <v>0.2593619821779376</v>
       </c>
       <c r="F24" t="n">
-        <v>0.003676157773431782</v>
+        <v>0.002450771848954521</v>
       </c>
       <c r="G24" t="n">
-        <v>0.01110882769371377</v>
+        <v>0.007405885129142515</v>
       </c>
       <c r="H24" t="n">
-        <v>1.229341126316166</v>
+        <v>0.8195607508774438</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.003118549765003491</v>
+        <v>0.002079033176668994</v>
       </c>
       <c r="B25" t="n">
-        <v>0.002639370233795065</v>
+        <v>0.001759580155863377</v>
       </c>
       <c r="C25" t="n">
-        <v>2.602207798737512</v>
+        <v>1.734805199158341</v>
       </c>
       <c r="D25" t="n">
-        <v>0.3260752281604024</v>
+        <v>0.2173834854402683</v>
       </c>
       <c r="E25" t="n">
-        <v>0.3638211912133695</v>
+        <v>0.242547460808913</v>
       </c>
       <c r="F25" t="n">
-        <v>0.003631902393739784</v>
+        <v>0.002421268262493189</v>
       </c>
       <c r="G25" t="n">
-        <v>0.01348368717168556</v>
+        <v>0.00898912478112371</v>
       </c>
       <c r="H25" t="n">
-        <v>1.215122838876736</v>
+        <v>0.8100818925844904</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.001994109353628874</v>
+        <v>0.001329406235752583</v>
       </c>
       <c r="B26" t="n">
-        <v>0.001500182461579962</v>
+        <v>0.001000121641053308</v>
       </c>
       <c r="C26" t="n">
-        <v>2.388274264464104</v>
+        <v>1.592182842976069</v>
       </c>
       <c r="D26" t="n">
-        <v>0.5054543470577899</v>
+        <v>0.3369695647051933</v>
       </c>
       <c r="E26" t="n">
-        <v>0.4295917518923772</v>
+        <v>0.2863945012615848</v>
       </c>
       <c r="F26" t="n">
-        <v>0.003715783851121192</v>
+        <v>0.002477189234080795</v>
       </c>
       <c r="G26" t="n">
-        <v>0.01219102111919664</v>
+        <v>0.008127347412797763</v>
       </c>
       <c r="H26" t="n">
-        <v>1.206919942224046</v>
+        <v>0.8046132948160307</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.002815876647768518</v>
+        <v>0.001877251098512345</v>
       </c>
       <c r="B27" t="n">
-        <v>0.001513145545857526</v>
+        <v>0.001008763697238351</v>
       </c>
       <c r="C27" t="n">
-        <v>2.386628568919796</v>
+        <v>1.591085712613197</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5009167932057197</v>
+        <v>0.3339445288038131</v>
       </c>
       <c r="E27" t="n">
-        <v>0.4137917262248509</v>
+        <v>0.2758611508165672</v>
       </c>
       <c r="F27" t="n">
-        <v>0.004088609409021909</v>
+        <v>0.002725739606014606</v>
       </c>
       <c r="G27" t="n">
-        <v>0.01100200971101854</v>
+        <v>0.007334673140679029</v>
       </c>
       <c r="H27" t="n">
-        <v>1.231141567079585</v>
+        <v>0.8207610447197231</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.003691172790463279</v>
+        <v>0.002460781860308853</v>
       </c>
       <c r="B28" t="n">
-        <v>0.008639229496363095</v>
+        <v>0.00575948633090873</v>
       </c>
       <c r="C28" t="n">
-        <v>2.312915923441131</v>
+        <v>1.541943948960754</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5295140626089734</v>
+        <v>0.3530093750726489</v>
       </c>
       <c r="E28" t="n">
-        <v>0.5158587573897541</v>
+        <v>0.3439058382598361</v>
       </c>
       <c r="F28" t="n">
-        <v>0.005558026850602152</v>
+        <v>0.003705351233734768</v>
       </c>
       <c r="G28" t="n">
-        <v>0.01088712794972892</v>
+        <v>0.007258085299819281</v>
       </c>
       <c r="H28" t="n">
-        <v>1.179390304161105</v>
+        <v>0.78626020277407</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.00271930888351851</v>
+        <v>0.00181287258901234</v>
       </c>
       <c r="B29" t="n">
-        <v>0.003214758104538675</v>
+        <v>0.00214317206969245</v>
       </c>
       <c r="C29" t="n">
-        <v>2.660525430678998</v>
+        <v>1.773683620452666</v>
       </c>
       <c r="D29" t="n">
-        <v>0.2503153932257894</v>
+        <v>0.1668769288171929</v>
       </c>
       <c r="E29" t="n">
-        <v>0.3771844901807923</v>
+        <v>0.2514563267871949</v>
       </c>
       <c r="F29" t="n">
-        <v>0.003619361631010351</v>
+        <v>0.002412907754006901</v>
       </c>
       <c r="G29" t="n">
-        <v>0.01218716326531291</v>
+        <v>0.008124775510208607</v>
       </c>
       <c r="H29" t="n">
-        <v>1.228879615089588</v>
+        <v>0.8192530767263918</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.002354701743475815</v>
+        <v>0.00156980116231721</v>
       </c>
       <c r="B30" t="n">
-        <v>0.00324767418641005</v>
+        <v>0.002165116124273367</v>
       </c>
       <c r="C30" t="n">
-        <v>2.647989042278101</v>
+        <v>1.765326028185401</v>
       </c>
       <c r="D30" t="n">
-        <v>0.2755288427225931</v>
+        <v>0.1836858951483954</v>
       </c>
       <c r="E30" t="n">
-        <v>0.3620105876926465</v>
+        <v>0.2413403917950976</v>
       </c>
       <c r="F30" t="n">
-        <v>0.004653626053036742</v>
+        <v>0.003102417368691161</v>
       </c>
       <c r="G30" t="n">
-        <v>0.01294333025175288</v>
+        <v>0.008628886834501918</v>
       </c>
       <c r="H30" t="n">
-        <v>1.22391087664175</v>
+        <v>0.8159405844278333</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.003137869686057822</v>
+        <v>0.002091913124038548</v>
       </c>
       <c r="B31" t="n">
-        <v>0.006196683640042031</v>
+        <v>0.004131122426694687</v>
       </c>
       <c r="C31" t="n">
-        <v>2.595677394125872</v>
+        <v>1.730451596083914</v>
       </c>
       <c r="D31" t="n">
-        <v>0.2973945264939703</v>
+        <v>0.1982630176626469</v>
       </c>
       <c r="E31" t="n">
-        <v>0.4015017471904969</v>
+        <v>0.2676678314603312</v>
       </c>
       <c r="F31" t="n">
-        <v>0.004318839457047023</v>
+        <v>0.002879226304698015</v>
       </c>
       <c r="G31" t="n">
-        <v>0.01325170403555821</v>
+        <v>0.008834469357038806</v>
       </c>
       <c r="H31" t="n">
-        <v>1.222650721734935</v>
+        <v>0.8151004811566237</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.001577767756431299</v>
+        <v>0.0010518451709542</v>
       </c>
       <c r="B32" t="n">
-        <v>0.002670672951189369</v>
+        <v>0.001780448634126246</v>
       </c>
       <c r="C32" t="n">
-        <v>2.647480994931902</v>
+        <v>1.764987329954602</v>
       </c>
       <c r="D32" t="n">
-        <v>0.2672596248214678</v>
+        <v>0.1781730832143118</v>
       </c>
       <c r="E32" t="n">
-        <v>0.3842997620808834</v>
+        <v>0.2561998413872556</v>
       </c>
       <c r="F32" t="n">
-        <v>0.00367497646223508</v>
+        <v>0.00244998430815672</v>
       </c>
       <c r="G32" t="n">
-        <v>0.01364360261043839</v>
+        <v>0.009095735073625592</v>
       </c>
       <c r="H32" t="n">
-        <v>1.217773847801146</v>
+        <v>0.8118492318674305</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.002766201591661115</v>
+        <v>0.001844134394440743</v>
       </c>
       <c r="B33" t="n">
-        <v>0.002378323280990597</v>
+        <v>0.001585548853993731</v>
       </c>
       <c r="C33" t="n">
-        <v>2.535012813081869</v>
+        <v>1.690008542054579</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3774176172523461</v>
+        <v>0.2516117448348974</v>
       </c>
       <c r="E33" t="n">
-        <v>0.3704695386627764</v>
+        <v>0.2469796924418509</v>
       </c>
       <c r="F33" t="n">
-        <v>0.004351188827537255</v>
+        <v>0.002900792551691503</v>
       </c>
       <c r="G33" t="n">
-        <v>0.01207944287169297</v>
+        <v>0.008052961914461983</v>
       </c>
       <c r="H33" t="n">
-        <v>1.234165134391369</v>
+        <v>0.8227767562609124</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.002041937547114838</v>
+        <v>0.001361291698076558</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0006144655788808654</v>
+        <v>0.0004096437192539102</v>
       </c>
       <c r="C34" t="n">
-        <v>2.311751110500392</v>
+        <v>1.541167407000261</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5953917529248739</v>
+        <v>0.3969278352832493</v>
       </c>
       <c r="E34" t="n">
-        <v>0.4439938025062386</v>
+        <v>0.2959958683374924</v>
       </c>
       <c r="F34" t="n">
-        <v>0.004150806500753089</v>
+        <v>0.002767204333835392</v>
       </c>
       <c r="G34" t="n">
-        <v>0.01084086437698529</v>
+        <v>0.007227242917990193</v>
       </c>
       <c r="H34" t="n">
-        <v>1.174987425226134</v>
+        <v>0.7833249501507559</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.001933719955237608</v>
+        <v>0.001289146636825072</v>
       </c>
       <c r="B35" t="n">
-        <v>0.003200452405373951</v>
+        <v>0.002133634936915968</v>
       </c>
       <c r="C35" t="n">
-        <v>2.667374099019438</v>
+        <v>1.778249399346292</v>
       </c>
       <c r="D35" t="n">
-        <v>0.2543995555749173</v>
+        <v>0.1695997037166116</v>
       </c>
       <c r="E35" t="n">
-        <v>0.3603046529218387</v>
+        <v>0.2402031019478925</v>
       </c>
       <c r="F35" t="n">
-        <v>0.004258392796191088</v>
+        <v>0.002838928530794058</v>
       </c>
       <c r="G35" t="n">
-        <v>0.01275513184515661</v>
+        <v>0.00850342123010441</v>
       </c>
       <c r="H35" t="n">
-        <v>1.229752995824059</v>
+        <v>0.8198353305493726</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.001944957513307245</v>
+        <v>0.00129663834220483</v>
       </c>
       <c r="B36" t="n">
-        <v>0.003511692449169149</v>
+        <v>0.002341128299446099</v>
       </c>
       <c r="C36" t="n">
-        <v>2.571012315858711</v>
+        <v>1.714008210572474</v>
       </c>
       <c r="D36" t="n">
-        <v>0.3195399106005006</v>
+        <v>0.2130266070670004</v>
       </c>
       <c r="E36" t="n">
-        <v>0.4290876502333381</v>
+        <v>0.286058433488892</v>
       </c>
       <c r="F36" t="n">
-        <v>0.004283139883379646</v>
+        <v>0.002855426588919764</v>
       </c>
       <c r="G36" t="n">
-        <v>0.01314216530666108</v>
+        <v>0.008761443537774053</v>
       </c>
       <c r="H36" t="n">
-        <v>1.20674540496285</v>
+        <v>0.8044969366419001</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.001319418195477075</v>
+        <v>0.0008796121303180504</v>
       </c>
       <c r="B37" t="n">
-        <v>0.002316084325933112</v>
+        <v>0.001544056217288741</v>
       </c>
       <c r="C37" t="n">
-        <v>1.634335531227855</v>
+        <v>1.08955702081857</v>
       </c>
       <c r="D37" t="n">
-        <v>1.180859813444094</v>
+        <v>0.7872398756293961</v>
       </c>
       <c r="E37" t="n">
-        <v>0.6837568796875663</v>
+        <v>0.4558379197917108</v>
       </c>
       <c r="F37" t="n">
-        <v>0.008195259059234161</v>
+        <v>0.00546350603948944</v>
       </c>
       <c r="G37" t="n">
-        <v>0.006014335575699474</v>
+        <v>0.004009557050466316</v>
       </c>
       <c r="H37" t="n">
-        <v>1.071969503626756</v>
+        <v>0.7146463357511708</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.002393885824894479</v>
+        <v>0.001595923883262986</v>
       </c>
       <c r="B38" t="n">
-        <v>0.001500780922151286</v>
+        <v>0.001000520614767524</v>
       </c>
       <c r="C38" t="n">
-        <v>2.550044884901196</v>
+        <v>1.700029923267464</v>
       </c>
       <c r="D38" t="n">
-        <v>0.3876801036896505</v>
+        <v>0.258453402459767</v>
       </c>
       <c r="E38" t="n">
-        <v>0.4150817778086686</v>
+        <v>0.276721185205779</v>
       </c>
       <c r="F38" t="n">
-        <v>0.005068999323947128</v>
+        <v>0.003379332882631419</v>
       </c>
       <c r="G38" t="n">
-        <v>0.01219588442459507</v>
+        <v>0.008130589616396712</v>
       </c>
       <c r="H38" t="n">
-        <v>1.153276522062429</v>
+        <v>0.7688510147082857</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.001572613792375659</v>
+        <v>0.001048409194917106</v>
       </c>
       <c r="B39" t="n">
-        <v>0.001478860490942634</v>
+        <v>0.0009859069939617557</v>
       </c>
       <c r="C39" t="n">
-        <v>2.64624643963264</v>
+        <v>1.764164293088427</v>
       </c>
       <c r="D39" t="n">
-        <v>0.2806850532013434</v>
+        <v>0.1871233688008956</v>
       </c>
       <c r="E39" t="n">
-        <v>0.4054023581748274</v>
+        <v>0.2702682387832183</v>
       </c>
       <c r="F39" t="n">
-        <v>0.003662971719132378</v>
+        <v>0.002441981146088252</v>
       </c>
       <c r="G39" t="n">
-        <v>0.01170149452428088</v>
+        <v>0.007800996349520585</v>
       </c>
       <c r="H39" t="n">
-        <v>1.182732987764149</v>
+        <v>0.7884886585094324</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.001620340740108921</v>
+        <v>0.001080227160072614</v>
       </c>
       <c r="B40" t="n">
-        <v>0.001523742138107498</v>
+        <v>0.001015828092071666</v>
       </c>
       <c r="C40" t="n">
-        <v>2.333161153238465</v>
+        <v>1.555440768825644</v>
       </c>
       <c r="D40" t="n">
-        <v>0.6014664337155876</v>
+        <v>0.4009776224770585</v>
       </c>
       <c r="E40" t="n">
-        <v>0.4214323265124004</v>
+        <v>0.2809548843416003</v>
       </c>
       <c r="F40" t="n">
-        <v>0.004460345535276145</v>
+        <v>0.002973563690184097</v>
       </c>
       <c r="G40" t="n">
-        <v>0.009449783939213583</v>
+        <v>0.006299855959475722</v>
       </c>
       <c r="H40" t="n">
-        <v>1.156427997825598</v>
+        <v>0.7709519985503985</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.001604571445131089</v>
+        <v>0.00106971429675406</v>
       </c>
       <c r="B41" t="n">
-        <v>0.003621391077611391</v>
+        <v>0.002414260718407594</v>
       </c>
       <c r="C41" t="n">
-        <v>2.34402170044463</v>
+        <v>1.562681133629754</v>
       </c>
       <c r="D41" t="n">
-        <v>0.5626290222597593</v>
+        <v>0.3750860148398396</v>
       </c>
       <c r="E41" t="n">
-        <v>0.4414851116215676</v>
+        <v>0.2943234077477118</v>
       </c>
       <c r="F41" t="n">
-        <v>0.00475670146020186</v>
+        <v>0.003171134306801241</v>
       </c>
       <c r="G41" t="n">
-        <v>0.01064855132593776</v>
+        <v>0.007099034217291837</v>
       </c>
       <c r="H41" t="n">
-        <v>1.172681626490223</v>
+        <v>0.7817877509934822</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.002732335395063027</v>
+        <v>0.001821556930042018</v>
       </c>
       <c r="B42" t="n">
-        <v>0.002642856548772745</v>
+        <v>0.001761904365848497</v>
       </c>
       <c r="C42" t="n">
-        <v>2.664989695825425</v>
+        <v>1.77665979721695</v>
       </c>
       <c r="D42" t="n">
-        <v>0.2851526333548807</v>
+        <v>0.1901017555699205</v>
       </c>
       <c r="E42" t="n">
-        <v>0.3528765242398992</v>
+        <v>0.2352510161599328</v>
       </c>
       <c r="F42" t="n">
-        <v>0.004297917866840465</v>
+        <v>0.002865278577893644</v>
       </c>
       <c r="G42" t="n">
-        <v>0.01224554435763115</v>
+        <v>0.008163696238420771</v>
       </c>
       <c r="H42" t="n">
-        <v>1.194616135877499</v>
+        <v>0.7964107572516661</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.001563773871700327</v>
+        <v>0.001042515914466885</v>
       </c>
       <c r="B43" t="n">
-        <v>0.0008823285437930014</v>
+        <v>0.0005882190291953344</v>
       </c>
       <c r="C43" t="n">
-        <v>2.66546731877789</v>
+        <v>1.776978212518594</v>
       </c>
       <c r="D43" t="n">
-        <v>0.2757072984747801</v>
+        <v>0.1838048656498534</v>
       </c>
       <c r="E43" t="n">
-        <v>0.3602936937593069</v>
+        <v>0.240195795839538</v>
       </c>
       <c r="F43" t="n">
-        <v>0.00264900476573215</v>
+        <v>0.001766003177154766</v>
       </c>
       <c r="G43" t="n">
-        <v>0.01226467625649822</v>
+        <v>0.00817645083766548</v>
       </c>
       <c r="H43" t="n">
-        <v>1.20813849450847</v>
+        <v>0.8054256630056469</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.002377750422455462</v>
+        <v>0.001585166948303641</v>
       </c>
       <c r="B44" t="n">
-        <v>0.004770128880231776</v>
+        <v>0.003180085920154517</v>
       </c>
       <c r="C44" t="n">
-        <v>2.533323988734333</v>
+        <v>1.688882659156222</v>
       </c>
       <c r="D44" t="n">
-        <v>0.3665813161915183</v>
+        <v>0.2443875441276789</v>
       </c>
       <c r="E44" t="n">
-        <v>0.4368089542097973</v>
+        <v>0.2912059694731982</v>
       </c>
       <c r="F44" t="n">
-        <v>0.004699177441141392</v>
+        <v>0.003132784960760928</v>
       </c>
       <c r="G44" t="n">
-        <v>0.01338880536639454</v>
+        <v>0.008925870244263022</v>
       </c>
       <c r="H44" t="n">
-        <v>1.180949346988515</v>
+        <v>0.7872995646590097</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.001938687056609284</v>
+        <v>0.001292458037739523</v>
       </c>
       <c r="B45" t="n">
-        <v>0.002041883030002603</v>
+        <v>0.001361255353335069</v>
       </c>
       <c r="C45" t="n">
-        <v>2.686107106323203</v>
+        <v>1.790738070882135</v>
       </c>
       <c r="D45" t="n">
-        <v>0.2501481599025208</v>
+        <v>0.1667654399350139</v>
       </c>
       <c r="E45" t="n">
-        <v>0.3560419341786</v>
+        <v>0.2373612894524</v>
       </c>
       <c r="F45" t="n">
-        <v>0.00361251104119095</v>
+        <v>0.0024083406941273</v>
       </c>
       <c r="G45" t="n">
-        <v>0.01185219597291735</v>
+        <v>0.007901463981944901</v>
       </c>
       <c r="H45" t="n">
-        <v>1.216149319295484</v>
+        <v>0.8107662128636557</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.001948711966086159</v>
+        <v>0.001299141310724106</v>
       </c>
       <c r="B46" t="n">
-        <v>0.002932059376656975</v>
+        <v>0.001954706251104651</v>
       </c>
       <c r="C46" t="n">
-        <v>2.557142360014752</v>
+        <v>1.704761573343168</v>
       </c>
       <c r="D46" t="n">
-        <v>0.3632962374587638</v>
+        <v>0.2421974916391759</v>
       </c>
       <c r="E46" t="n">
-        <v>0.3842842257886536</v>
+        <v>0.2561894838591025</v>
       </c>
       <c r="F46" t="n">
-        <v>0.004621516147615392</v>
+        <v>0.003081010765076928</v>
       </c>
       <c r="G46" t="n">
-        <v>0.0115999707041159</v>
+        <v>0.007733313802743932</v>
       </c>
       <c r="H46" t="n">
-        <v>1.209074848463855</v>
+        <v>0.8060498989759032</v>
       </c>
     </row>
     <row r="47">
@@ -1651,77 +1651,77 @@
         <v>1e-07</v>
       </c>
       <c r="B47" t="n">
-        <v>0.00201281013949921</v>
+        <v>0.001341873426332806</v>
       </c>
       <c r="C47" t="n">
-        <v>2.738856479537054</v>
+        <v>1.825904319691369</v>
       </c>
       <c r="D47" t="n">
-        <v>0.2405426954877732</v>
+        <v>0.1603617969918488</v>
       </c>
       <c r="E47" t="n">
-        <v>0.3627994540411039</v>
+        <v>0.2418663026940693</v>
       </c>
       <c r="F47" t="n">
-        <v>0.002913606915029109</v>
+        <v>0.001942404610019406</v>
       </c>
       <c r="G47" t="n">
-        <v>0.01076106422315003</v>
+        <v>0.007174042815433351</v>
       </c>
       <c r="H47" t="n">
-        <v>1.150401492004479</v>
+        <v>0.7669343280029862</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.002312585227490926</v>
+        <v>0.00154172348499395</v>
       </c>
       <c r="B48" t="n">
-        <v>0.0008698870482898471</v>
+        <v>0.0005799246988598981</v>
       </c>
       <c r="C48" t="n">
-        <v>2.703743303829001</v>
+        <v>1.802495535886001</v>
       </c>
       <c r="D48" t="n">
-        <v>0.2593256673137749</v>
+        <v>0.1728837782091833</v>
       </c>
       <c r="E48" t="n">
-        <v>0.3832564357671902</v>
+        <v>0.2555042905114601</v>
       </c>
       <c r="F48" t="n">
-        <v>0.004570390663844261</v>
+        <v>0.003046927109229508</v>
       </c>
       <c r="G48" t="n">
-        <v>0.0114716461251171</v>
+        <v>0.007647764083411402</v>
       </c>
       <c r="H48" t="n">
-        <v>1.149733126178121</v>
+        <v>0.7664887507854139</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.000437742986682231</v>
+        <v>0.000291828657788154</v>
       </c>
       <c r="B49" t="n">
-        <v>0.007244976662045034</v>
+        <v>0.004829984441363355</v>
       </c>
       <c r="C49" t="n">
-        <v>1.798467595302741</v>
+        <v>1.198978396868494</v>
       </c>
       <c r="D49" t="n">
-        <v>1.161130862363981</v>
+        <v>0.7740872415759872</v>
       </c>
       <c r="E49" t="n">
-        <v>0.5414376796113429</v>
+        <v>0.3609584530742286</v>
       </c>
       <c r="F49" t="n">
-        <v>0.01038140226295442</v>
+        <v>0.006920934841969611</v>
       </c>
       <c r="G49" t="n">
-        <v>0.007394622573306353</v>
+        <v>0.004929748382204236</v>
       </c>
       <c r="H49" t="n">
-        <v>0.9860231697548587</v>
+        <v>0.6573487798365726</v>
       </c>
     </row>
     <row r="50">
@@ -1729,25 +1729,25 @@
         <v>1e-07</v>
       </c>
       <c r="B50" t="n">
-        <v>0.001167717017708827</v>
+        <v>0.0007784780118058846</v>
       </c>
       <c r="C50" t="n">
-        <v>2.711564833035442</v>
+        <v>1.807709888690295</v>
       </c>
       <c r="D50" t="n">
-        <v>0.282253788266816</v>
+        <v>0.1881691921778773</v>
       </c>
       <c r="E50" t="n">
-        <v>0.3654113227665122</v>
+        <v>0.2436075485110081</v>
       </c>
       <c r="F50" t="n">
-        <v>0.00493006398032667</v>
+        <v>0.003286709320217779</v>
       </c>
       <c r="G50" t="n">
-        <v>0.01030087140335448</v>
+        <v>0.006867247602236317</v>
       </c>
       <c r="H50" t="n">
-        <v>1.126294375861001</v>
+        <v>0.7508629172406674</v>
       </c>
     </row>
     <row r="51">
@@ -1755,25 +1755,25 @@
         <v>1e-07</v>
       </c>
       <c r="B51" t="n">
-        <v>0.001435424269302309</v>
+        <v>0.0009569495128682063</v>
       </c>
       <c r="C51" t="n">
-        <v>2.80104321117327</v>
+        <v>1.86736214078218</v>
       </c>
       <c r="D51" t="n">
-        <v>0.2051603952973535</v>
+        <v>0.1367735968649024</v>
       </c>
       <c r="E51" t="n">
-        <v>0.3456246659068502</v>
+        <v>0.2304164439379001</v>
       </c>
       <c r="F51" t="n">
-        <v>0.002585734593068868</v>
+        <v>0.001723823062045912</v>
       </c>
       <c r="G51" t="n">
-        <v>0.009822966573583584</v>
+        <v>0.006548644382389057</v>
       </c>
       <c r="H51" t="n">
-        <v>1.129790374681958</v>
+        <v>0.7531935831213055</v>
       </c>
     </row>
     <row r="52">
@@ -1781,25 +1781,25 @@
         <v>1e-07</v>
       </c>
       <c r="B52" t="n">
-        <v>0.002311704152474356</v>
+        <v>0.001541136101649571</v>
       </c>
       <c r="C52" t="n">
-        <v>2.788132408404426</v>
+        <v>1.858754938936284</v>
       </c>
       <c r="D52" t="n">
-        <v>0.2256344527203643</v>
+        <v>0.1504229684802428</v>
       </c>
       <c r="E52" t="n">
-        <v>0.3189756318767101</v>
+        <v>0.2126504212511401</v>
       </c>
       <c r="F52" t="n">
-        <v>0.004879970576110611</v>
+        <v>0.003253313717407073</v>
       </c>
       <c r="G52" t="n">
-        <v>0.009269278443676924</v>
+        <v>0.006179518962451282</v>
       </c>
       <c r="H52" t="n">
-        <v>1.141189877275727</v>
+        <v>0.7607932515171516</v>
       </c>
     </row>
     <row r="53">
@@ -1807,233 +1807,233 @@
         <v>1e-07</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0006077781707404804</v>
+        <v>0.0004051854471603202</v>
       </c>
       <c r="C53" t="n">
-        <v>2.289924178795069</v>
+        <v>1.526616119196713</v>
       </c>
       <c r="D53" t="n">
-        <v>0.7006902256872372</v>
+        <v>0.4671268171248247</v>
       </c>
       <c r="E53" t="n">
-        <v>0.4050422034116973</v>
+        <v>0.2700281356077982</v>
       </c>
       <c r="F53" t="n">
-        <v>0.005132040078469818</v>
+        <v>0.003421360052313212</v>
       </c>
       <c r="G53" t="n">
-        <v>0.005523907923908879</v>
+        <v>0.003682605282605919</v>
       </c>
       <c r="H53" t="n">
-        <v>1.097164685520983</v>
+        <v>0.731443123680655</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0.003533649291925376</v>
+        <v>0.002355766194616917</v>
       </c>
       <c r="B54" t="n">
-        <v>0.007679790911852031</v>
+        <v>0.005119860607901353</v>
       </c>
       <c r="C54" t="n">
-        <v>2.528410954343292</v>
+        <v>1.685607302895528</v>
       </c>
       <c r="D54" t="n">
-        <v>0.3635023956065637</v>
+        <v>0.2423349304043757</v>
       </c>
       <c r="E54" t="n">
-        <v>0.4402303686389042</v>
+        <v>0.2934869124259361</v>
       </c>
       <c r="F54" t="n">
-        <v>0.003990625492230239</v>
+        <v>0.002660416994820159</v>
       </c>
       <c r="G54" t="n">
-        <v>0.009475010728804172</v>
+        <v>0.00631667381920278</v>
       </c>
       <c r="H54" t="n">
-        <v>1.178224824855521</v>
+        <v>0.7854832165703476</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0.003602014133028398</v>
+        <v>0.002401342755352266</v>
       </c>
       <c r="B55" t="n">
-        <v>0.00903273503849184</v>
+        <v>0.006021823358994561</v>
       </c>
       <c r="C55" t="n">
-        <v>2.451385751700217</v>
+        <v>1.634257167800145</v>
       </c>
       <c r="D55" t="n">
-        <v>0.4151510927808749</v>
+        <v>0.2767673951872499</v>
       </c>
       <c r="E55" t="n">
-        <v>0.496407871841677</v>
+        <v>0.3309385812277846</v>
       </c>
       <c r="F55" t="n">
-        <v>0.004745803259177445</v>
+        <v>0.00316386883945163</v>
       </c>
       <c r="G55" t="n">
-        <v>0.009014433829493665</v>
+        <v>0.006009622552995778</v>
       </c>
       <c r="H55" t="n">
-        <v>1.154482439913414</v>
+        <v>0.769654959942276</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0.003194261426071625</v>
+        <v>0.002129507617381083</v>
       </c>
       <c r="B56" t="n">
-        <v>0.003904981093743504</v>
+        <v>0.002603320729162336</v>
       </c>
       <c r="C56" t="n">
-        <v>2.366563397497829</v>
+        <v>1.577708931665219</v>
       </c>
       <c r="D56" t="n">
-        <v>0.5322399719993671</v>
+        <v>0.354826647999578</v>
       </c>
       <c r="E56" t="n">
-        <v>0.4657613159089395</v>
+        <v>0.310507543939293</v>
       </c>
       <c r="F56" t="n">
-        <v>0.005072832476246391</v>
+        <v>0.003381888317497594</v>
       </c>
       <c r="G56" t="n">
-        <v>0.009635610704425918</v>
+        <v>0.006423740469617278</v>
       </c>
       <c r="H56" t="n">
-        <v>1.145815421020939</v>
+        <v>0.7638769473472924</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0.002894654053819302</v>
+        <v>0.001929769369212868</v>
       </c>
       <c r="B57" t="n">
-        <v>0.008399578730038867</v>
+        <v>0.005599719153359245</v>
       </c>
       <c r="C57" t="n">
-        <v>2.282332019261727</v>
+        <v>1.521554679507818</v>
       </c>
       <c r="D57" t="n">
-        <v>0.5453359410259251</v>
+        <v>0.3635572940172834</v>
       </c>
       <c r="E57" t="n">
-        <v>0.6234511293375304</v>
+        <v>0.4156340862250203</v>
       </c>
       <c r="F57" t="n">
-        <v>0.005954240063649289</v>
+        <v>0.003969493375766193</v>
       </c>
       <c r="G57" t="n">
-        <v>0.006985466964961111</v>
+        <v>0.004656977976640741</v>
       </c>
       <c r="H57" t="n">
-        <v>1.084346111155166</v>
+        <v>0.722897407436777</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0.001561990287927877</v>
+        <v>0.001041326858618585</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0002937740639503244</v>
+        <v>0.000195849375966883</v>
       </c>
       <c r="C58" t="n">
-        <v>2.510551475453406</v>
+        <v>1.673700983635605</v>
       </c>
       <c r="D58" t="n">
-        <v>0.4238950278333317</v>
+        <v>0.2825966852222211</v>
       </c>
       <c r="E58" t="n">
-        <v>0.3585948197097161</v>
+        <v>0.2390632131398107</v>
       </c>
       <c r="F58" t="n">
-        <v>0.00463047096217062</v>
+        <v>0.00308698064144708</v>
       </c>
       <c r="G58" t="n">
-        <v>0.0109942068308352</v>
+        <v>0.007329471220556803</v>
       </c>
       <c r="H58" t="n">
-        <v>1.211999727456618</v>
+        <v>0.8079998183044118</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>0.001543485722355212</v>
+        <v>0.001028990481570142</v>
       </c>
       <c r="B59" t="n">
-        <v>0.002612644067821994</v>
+        <v>0.001741762711881329</v>
       </c>
       <c r="C59" t="n">
-        <v>2.681821020773123</v>
+        <v>1.787880680515415</v>
       </c>
       <c r="D59" t="n">
-        <v>0.2599271633576789</v>
+        <v>0.173284775571786</v>
       </c>
       <c r="E59" t="n">
-        <v>0.335307114524045</v>
+        <v>0.2235380763493634</v>
       </c>
       <c r="F59" t="n">
-        <v>0.002941466632034108</v>
+        <v>0.001960977754689406</v>
       </c>
       <c r="G59" t="n">
-        <v>0.01241595521023245</v>
+        <v>0.008277303473488304</v>
       </c>
       <c r="H59" t="n">
-        <v>1.221226102801567</v>
+        <v>0.8141507352010448</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0.001524667804609907</v>
+        <v>0.001016445203073271</v>
       </c>
       <c r="B60" t="n">
-        <v>0.003154300296588454</v>
+        <v>0.002102866864392303</v>
       </c>
       <c r="C60" t="n">
-        <v>2.65766013057746</v>
+        <v>1.771773420384974</v>
       </c>
       <c r="D60" t="n">
-        <v>0.2856886738110963</v>
+        <v>0.1904591158740642</v>
       </c>
       <c r="E60" t="n">
-        <v>0.3428870792432241</v>
+        <v>0.2285913861621494</v>
       </c>
       <c r="F60" t="n">
-        <v>0.003874139688923003</v>
+        <v>0.002582759792615336</v>
       </c>
       <c r="G60" t="n">
-        <v>0.01287781107609863</v>
+        <v>0.008585207384065754</v>
       </c>
       <c r="H60" t="n">
-        <v>1.210882902851004</v>
+        <v>0.807255268567336</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>0.003538687404551622</v>
+        <v>0.002359124936367748</v>
       </c>
       <c r="B61" t="n">
-        <v>0.003549572492375469</v>
+        <v>0.002366381661583646</v>
       </c>
       <c r="C61" t="n">
-        <v>2.634890573647056</v>
+        <v>1.756593715764704</v>
       </c>
       <c r="D61" t="n">
-        <v>0.3015371823952828</v>
+        <v>0.2010247882635219</v>
       </c>
       <c r="E61" t="n">
-        <v>0.3291040099789594</v>
+        <v>0.2194026733193062</v>
       </c>
       <c r="F61" t="n">
-        <v>0.004662367663619286</v>
+        <v>0.003108245109079525</v>
       </c>
       <c r="G61" t="n">
-        <v>0.01170250770144055</v>
+        <v>0.007801671800960369</v>
       </c>
       <c r="H61" t="n">
-        <v>1.228554503459285</v>
+        <v>0.819036335639523</v>
       </c>
     </row>
     <row r="62">
@@ -2041,51 +2041,51 @@
         <v>1e-07</v>
       </c>
       <c r="B62" t="n">
-        <v>0.001427010867294102</v>
+        <v>0.0009513405781960678</v>
       </c>
       <c r="C62" t="n">
-        <v>2.812346618324735</v>
+        <v>1.874897745549823</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1493691649063783</v>
+        <v>0.09957944327091887</v>
       </c>
       <c r="E62" t="n">
-        <v>0.3033061107625409</v>
+        <v>0.2022040738416939</v>
       </c>
       <c r="F62" t="n">
-        <v>0.003213223646797678</v>
+        <v>0.002142149097865119</v>
       </c>
       <c r="G62" t="n">
-        <v>0.002746516377250552</v>
+        <v>0.001831010918167034</v>
       </c>
       <c r="H62" t="n">
-        <v>1.233449256554005</v>
+        <v>0.8222995043693366</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>0.00614103463870991</v>
+        <v>0.004094023092473273</v>
       </c>
       <c r="B63" t="n">
-        <v>0.003176211126724537</v>
+        <v>0.002117474084483025</v>
       </c>
       <c r="C63" t="n">
-        <v>2.572532263865615</v>
+        <v>1.715021509243743</v>
       </c>
       <c r="D63" t="n">
-        <v>0.3480602514611714</v>
+        <v>0.2320401676407809</v>
       </c>
       <c r="E63" t="n">
-        <v>0.3383165787542091</v>
+        <v>0.2255443858361394</v>
       </c>
       <c r="F63" t="n">
-        <v>0.006501751275737759</v>
+        <v>0.004334500850491839</v>
       </c>
       <c r="G63" t="n">
         <v>1e-07</v>
       </c>
       <c r="H63" t="n">
-        <v>1.247902598586651</v>
+        <v>0.8319350657244338</v>
       </c>
     </row>
     <row r="64">
@@ -2096,13 +2096,13 @@
         <v>1e-07</v>
       </c>
       <c r="C64" t="n">
-        <v>2.29487197320092</v>
+        <v>1.529914648800614</v>
       </c>
       <c r="D64" t="n">
-        <v>0.4143880746874763</v>
+        <v>0.2762587164583176</v>
       </c>
       <c r="E64" t="n">
-        <v>0.4343094068721252</v>
+        <v>0.2895396045814168</v>
       </c>
       <c r="F64" t="n">
         <v>1e-07</v>
@@ -2111,85 +2111,85 @@
         <v>1e-07</v>
       </c>
       <c r="H64" t="n">
-        <v>1.501800521295279</v>
+        <v>1.001200347530186</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>0.006639603224792381</v>
+        <v>0.004426402149861588</v>
       </c>
       <c r="B65" t="n">
-        <v>0.002350597695700911</v>
+        <v>0.001567065130467274</v>
       </c>
       <c r="C65" t="n">
-        <v>2.57634815063201</v>
+        <v>1.717565433754674</v>
       </c>
       <c r="D65" t="n">
-        <v>0.385369410350432</v>
+        <v>0.2569129402336213</v>
       </c>
       <c r="E65" t="n">
-        <v>0.3393671946872255</v>
+        <v>0.2262447964581503</v>
       </c>
       <c r="F65" t="n">
-        <v>0.01058575834710536</v>
+        <v>0.007057172231403574</v>
       </c>
       <c r="G65" t="n">
         <v>1e-07</v>
       </c>
       <c r="H65" t="n">
-        <v>1.182514809225784</v>
+        <v>0.788343206150523</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>0.01592608830557687</v>
+        <v>0.01061739220371792</v>
       </c>
       <c r="B66" t="n">
-        <v>0.003214497269112276</v>
+        <v>0.002142998179408184</v>
       </c>
       <c r="C66" t="n">
-        <v>2.633299021148953</v>
+        <v>1.755532680765969</v>
       </c>
       <c r="D66" t="n">
-        <v>0.3034252054184305</v>
+        <v>0.2022834702789537</v>
       </c>
       <c r="E66" t="n">
-        <v>0.3615609610653722</v>
+        <v>0.2410406407102482</v>
       </c>
       <c r="F66" t="n">
-        <v>0.006580123576942202</v>
+        <v>0.004386749051294801</v>
       </c>
       <c r="G66" t="n">
         <v>1e-07</v>
       </c>
       <c r="H66" t="n">
-        <v>1.177242955809543</v>
+        <v>0.7848286372063624</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>0.002796328555424331</v>
+        <v>0.001864219036949554</v>
       </c>
       <c r="B67" t="n">
-        <v>0.001502641140814053</v>
+        <v>0.001001760760542702</v>
       </c>
       <c r="C67" t="n">
-        <v>2.573921331380896</v>
+        <v>1.71594755425393</v>
       </c>
       <c r="D67" t="n">
-        <v>0.4544858839765865</v>
+        <v>0.3029905893177243</v>
       </c>
       <c r="E67" t="n">
-        <v>0.2508945339013609</v>
+        <v>0.1672630226009072</v>
       </c>
       <c r="F67" t="n">
-        <v>0.002030112940402571</v>
+        <v>0.001353408626935047</v>
       </c>
       <c r="G67" t="n">
         <v>1e-07</v>
       </c>
       <c r="H67" t="n">
-        <v>1.179122175109202</v>
+        <v>0.7860814500728011</v>
       </c>
     </row>
     <row r="68">
@@ -2200,13 +2200,13 @@
         <v>1e-07</v>
       </c>
       <c r="C68" t="n">
-        <v>2.7357353460308</v>
+        <v>1.823823564020534</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2017587838819546</v>
+        <v>0.1345058559213031</v>
       </c>
       <c r="E68" t="n">
-        <v>0.3537683316249228</v>
+        <v>0.2358455544166152</v>
       </c>
       <c r="F68" t="n">
         <v>1e-07</v>
@@ -2215,33 +2215,33 @@
         <v>1e-07</v>
       </c>
       <c r="H68" t="n">
-        <v>1.230947437545248</v>
+        <v>0.8206316250301656</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>0.004357255336054616</v>
+        <v>0.002904836890703077</v>
       </c>
       <c r="B69" t="n">
-        <v>0.007747985272033383</v>
+        <v>0.005165323514688922</v>
       </c>
       <c r="C69" t="n">
-        <v>2.492039560353106</v>
+        <v>1.661359706902071</v>
       </c>
       <c r="D69" t="n">
-        <v>0.4531670282351501</v>
+        <v>0.3021113521567668</v>
       </c>
       <c r="E69" t="n">
-        <v>0.3899041818677988</v>
+        <v>0.2599361212451992</v>
       </c>
       <c r="F69" t="n">
-        <v>0.00335505092682969</v>
+        <v>0.002236700617886461</v>
       </c>
       <c r="G69" t="n">
         <v>1e-07</v>
       </c>
       <c r="H69" t="n">
-        <v>1.155028325473374</v>
+        <v>0.7700188836489159</v>
       </c>
     </row>
     <row r="70">
@@ -2249,42 +2249,42 @@
         <v>1e-07</v>
       </c>
       <c r="B70" t="n">
-        <v>0.003788160474272668</v>
+        <v>0.002525440316181778</v>
       </c>
       <c r="C70" t="n">
-        <v>2.660057095635972</v>
+        <v>1.773371397090648</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2802079443949382</v>
+        <v>0.1868052962632921</v>
       </c>
       <c r="E70" t="n">
-        <v>0.3462810398823025</v>
+        <v>0.2308540265882016</v>
       </c>
       <c r="F70" t="n">
-        <v>0.003280716435035926</v>
+        <v>0.002187144290023951</v>
       </c>
       <c r="G70" t="n">
-        <v>0.004050519952307966</v>
+        <v>0.002700346634871977</v>
       </c>
       <c r="H70" t="n">
-        <v>1.216050830612381</v>
+        <v>0.8107005537415874</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>0.01070803545418051</v>
+        <v>0.007138690302787007</v>
       </c>
       <c r="B71" t="n">
-        <v>0.004315569761876251</v>
+        <v>0.002877046507917502</v>
       </c>
       <c r="C71" t="n">
-        <v>2.71424194657616</v>
+        <v>1.809494631050774</v>
       </c>
       <c r="D71" t="n">
-        <v>0.2567017956987041</v>
+        <v>0.1711345304658028</v>
       </c>
       <c r="E71" t="n">
-        <v>0.3019151236999063</v>
+        <v>0.2012767491332709</v>
       </c>
       <c r="F71" t="n">
         <v>1e-07</v>
@@ -2293,33 +2293,33 @@
         <v>1e-07</v>
       </c>
       <c r="H71" t="n">
-        <v>1.202352492356439</v>
+        <v>0.8015683282376258</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>0.01036106799709693</v>
+        <v>0.006907378664731284</v>
       </c>
       <c r="B72" t="n">
-        <v>0.00404169845808044</v>
+        <v>0.002694465638720293</v>
       </c>
       <c r="C72" t="n">
-        <v>2.70004578409939</v>
+        <v>1.800030522732926</v>
       </c>
       <c r="D72" t="n">
-        <v>0.2706294540491164</v>
+        <v>0.1804196360327442</v>
       </c>
       <c r="E72" t="n">
-        <v>0.3161098984747462</v>
+        <v>0.2107399323164975</v>
       </c>
       <c r="F72" t="n">
-        <v>0.006825568758643464</v>
+        <v>0.004550379172428975</v>
       </c>
       <c r="G72" t="n">
         <v>1e-07</v>
       </c>
       <c r="H72" t="n">
-        <v>1.18245519991271</v>
+        <v>0.7883034666084736</v>
       </c>
     </row>
     <row r="73">
@@ -2327,16 +2327,16 @@
         <v>1e-07</v>
       </c>
       <c r="B73" t="n">
-        <v>0.004271372486746518</v>
+        <v>0.002847581657831012</v>
       </c>
       <c r="C73" t="n">
-        <v>2.257450728707326</v>
+        <v>1.504967152471551</v>
       </c>
       <c r="D73" t="n">
-        <v>0.6691695851541138</v>
+        <v>0.4461130567694092</v>
       </c>
       <c r="E73" t="n">
-        <v>0.4263248812040089</v>
+        <v>0.2842165874693393</v>
       </c>
       <c r="F73" t="n">
         <v>1e-07</v>
@@ -2345,50 +2345,50 @@
         <v>1e-07</v>
       </c>
       <c r="H73" t="n">
-        <v>1.163800367269414</v>
+        <v>0.7758669115129426</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>0.01291091545001457</v>
+        <v>0.008607276966676384</v>
       </c>
       <c r="B74" t="n">
-        <v>0.01456945845457758</v>
+        <v>0.009712972303051719</v>
       </c>
       <c r="C74" t="n">
-        <v>2.22540443607326</v>
+        <v>1.483602957382173</v>
       </c>
       <c r="D74" t="n">
-        <v>0.6701971219125057</v>
+        <v>0.4467980812750038</v>
       </c>
       <c r="E74" t="n">
-        <v>0.3893802975294746</v>
+        <v>0.2595868650196497</v>
       </c>
       <c r="F74" t="n">
-        <v>0.007518107495749294</v>
+        <v>0.005012071663832863</v>
       </c>
       <c r="G74" t="n">
         <v>1e-07</v>
       </c>
       <c r="H74" t="n">
-        <v>1.196915784286779</v>
+        <v>0.797943856191186</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0.006168133269734121</v>
+        <v>0.004112088846489414</v>
       </c>
       <c r="B75" t="n">
-        <v>0.01299292385259148</v>
+        <v>0.008661949235060987</v>
       </c>
       <c r="C75" t="n">
-        <v>2.19105376289242</v>
+        <v>1.460702508594947</v>
       </c>
       <c r="D75" t="n">
-        <v>0.7282490976669581</v>
+        <v>0.4854993984446387</v>
       </c>
       <c r="E75" t="n">
-        <v>0.394101612871656</v>
+        <v>0.262734408581104</v>
       </c>
       <c r="F75" t="n">
         <v>1e-07</v>
@@ -2397,7 +2397,7 @@
         <v>1e-07</v>
       </c>
       <c r="H75" t="n">
-        <v>1.188621982044626</v>
+        <v>0.792414654696417</v>
       </c>
     </row>
     <row r="76">
@@ -2408,48 +2408,48 @@
         <v>1e-07</v>
       </c>
       <c r="C76" t="n">
-        <v>2.551977810235214</v>
+        <v>1.701318540156809</v>
       </c>
       <c r="D76" t="n">
-        <v>0.3807766280496622</v>
+        <v>0.2538510853664414</v>
       </c>
       <c r="E76" t="n">
-        <v>0.3569302267803011</v>
+        <v>0.2379534845202007</v>
       </c>
       <c r="F76" t="n">
         <v>1e-07</v>
       </c>
       <c r="G76" t="n">
-        <v>0.0006299458820443772</v>
+        <v>0.0004199639213629181</v>
       </c>
       <c r="H76" t="n">
-        <v>1.243308169910342</v>
+        <v>0.8288721132735614</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>0.006567909352134213</v>
+        <v>0.004378606234756142</v>
       </c>
       <c r="B77" t="n">
-        <v>0.00435978026453773</v>
+        <v>0.002906520176358487</v>
       </c>
       <c r="C77" t="n">
-        <v>2.689683862254299</v>
+        <v>1.793122574836199</v>
       </c>
       <c r="D77" t="n">
-        <v>0.2443642462387362</v>
+        <v>0.1629094974924908</v>
       </c>
       <c r="E77" t="n">
-        <v>0.3518578248714215</v>
+        <v>0.2345718832476143</v>
       </c>
       <c r="F77" t="n">
-        <v>0.002617863556506427</v>
+        <v>0.001745242371004285</v>
       </c>
       <c r="G77" t="n">
-        <v>0.01212049499479188</v>
+        <v>0.00808032999652792</v>
       </c>
       <c r="H77" t="n">
-        <v>1.210062327292857</v>
+        <v>0.8067082181952379</v>
       </c>
     </row>
     <row r="78">
@@ -2457,16 +2457,16 @@
         <v>1e-07</v>
       </c>
       <c r="B78" t="n">
-        <v>0.001508811783137304</v>
+        <v>0.001005874522091536</v>
       </c>
       <c r="C78" t="n">
-        <v>2.490415171280431</v>
+        <v>1.66027678085362</v>
       </c>
       <c r="D78" t="n">
-        <v>0.4417641948113172</v>
+        <v>0.2945094632075447</v>
       </c>
       <c r="E78" t="n">
-        <v>0.3663141482707108</v>
+        <v>0.2442094321804738</v>
       </c>
       <c r="F78" t="n">
         <v>1e-07</v>
@@ -2475,293 +2475,293 @@
         <v>1e-07</v>
       </c>
       <c r="H78" t="n">
-        <v>1.232399179025394</v>
+        <v>0.8215994526835958</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>0.01170437353626041</v>
+        <v>0.007802915690840276</v>
       </c>
       <c r="B79" t="n">
-        <v>0.003815622353274796</v>
+        <v>0.002543748235516531</v>
       </c>
       <c r="C79" t="n">
-        <v>2.655430535254041</v>
+        <v>1.770287023502694</v>
       </c>
       <c r="D79" t="n">
-        <v>0.2538611255956802</v>
+        <v>0.1692407503971202</v>
       </c>
       <c r="E79" t="n">
-        <v>0.3341088507430144</v>
+        <v>0.2227392338286762</v>
       </c>
       <c r="F79" t="n">
-        <v>0.001982699790459519</v>
+        <v>0.001321799860306346</v>
       </c>
       <c r="G79" t="n">
-        <v>0.01223965133793277</v>
+        <v>0.00815976755862185</v>
       </c>
       <c r="H79" t="n">
-        <v>1.256273298255699</v>
+        <v>0.8375155321704658</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0.006281036853072861</v>
+        <v>0.004187357902048573</v>
       </c>
       <c r="B80" t="n">
-        <v>0.005985339600259069</v>
+        <v>0.003990226400172712</v>
       </c>
       <c r="C80" t="n">
-        <v>2.098405307176398</v>
+        <v>1.398936871450932</v>
       </c>
       <c r="D80" t="n">
-        <v>0.8190477566487215</v>
+        <v>0.5460318377658144</v>
       </c>
       <c r="E80" t="n">
-        <v>0.3918603067527001</v>
+        <v>0.2612402045018</v>
       </c>
       <c r="F80" t="n">
-        <v>0.003546654423344439</v>
+        <v>0.002364436282229626</v>
       </c>
       <c r="G80" t="n">
-        <v>0.007410376675190461</v>
+        <v>0.00494025111679364</v>
       </c>
       <c r="H80" t="n">
-        <v>1.196021664281339</v>
+        <v>0.7973477761875595</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>0.0007771278525178577</v>
+        <v>0.0005180852350119052</v>
       </c>
       <c r="B81" t="n">
-        <v>0.002046235580916629</v>
+        <v>0.001364157053944419</v>
       </c>
       <c r="C81" t="n">
-        <v>2.651075315803661</v>
+        <v>1.767383543869107</v>
       </c>
       <c r="D81" t="n">
-        <v>0.3185742596836295</v>
+        <v>0.2123828397890864</v>
       </c>
       <c r="E81" t="n">
-        <v>0.3620001702145838</v>
+        <v>0.2413334468097226</v>
       </c>
       <c r="F81" t="n">
-        <v>0.004936652180402728</v>
+        <v>0.003291101453601819</v>
       </c>
       <c r="G81" t="n">
-        <v>0.006563859770922183</v>
+        <v>0.004375906513948122</v>
       </c>
       <c r="H81" t="n">
-        <v>1.164871469656263</v>
+        <v>0.7765809797708418</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>0.0007797825496224501</v>
+        <v>0.0005198550330816334</v>
       </c>
       <c r="B82" t="n">
-        <v>0.00322649736567096</v>
+        <v>0.00215099824378064</v>
       </c>
       <c r="C82" t="n">
-        <v>2.671159842309923</v>
+        <v>1.780773228206615</v>
       </c>
       <c r="D82" t="n">
-        <v>0.2496881793581258</v>
+        <v>0.1664587862387505</v>
       </c>
       <c r="E82" t="n">
-        <v>0.3893220022909708</v>
+        <v>0.2595480015273139</v>
       </c>
       <c r="F82" t="n">
-        <v>0.004623281566781225</v>
+        <v>0.003082187711187483</v>
       </c>
       <c r="G82" t="n">
-        <v>0.01129076940932606</v>
+        <v>0.007527179606217373</v>
       </c>
       <c r="H82" t="n">
-        <v>1.20430565766198</v>
+        <v>0.8028704384413198</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>0.004309367859401679</v>
+        <v>0.002872911906267786</v>
       </c>
       <c r="B83" t="n">
-        <v>0.003241967684172429</v>
+        <v>0.002161311789448287</v>
       </c>
       <c r="C83" t="n">
-        <v>2.565767604855191</v>
+        <v>1.710511736570128</v>
       </c>
       <c r="D83" t="n">
-        <v>0.4017263385425274</v>
+        <v>0.2678175590283516</v>
       </c>
       <c r="E83" t="n">
-        <v>0.3472864616292586</v>
+        <v>0.231524307752839</v>
       </c>
       <c r="F83" t="n">
-        <v>0.004645449146746134</v>
+        <v>0.003096966097830756</v>
       </c>
       <c r="G83" t="n">
-        <v>0.005987589315677218</v>
+        <v>0.003991726210451479</v>
       </c>
       <c r="H83" t="n">
-        <v>1.172119023684852</v>
+        <v>0.7814126824565683</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>0.00250724556237978</v>
+        <v>0.00167149704158652</v>
       </c>
       <c r="B84" t="n">
-        <v>0.004715546081652298</v>
+        <v>0.003143697387768199</v>
       </c>
       <c r="C84" t="n">
-        <v>2.088670490958303</v>
+        <v>1.392446993972202</v>
       </c>
       <c r="D84" t="n">
-        <v>0.7972093619830652</v>
+        <v>0.5314729079887102</v>
       </c>
       <c r="E84" t="n">
-        <v>0.499738447720023</v>
+        <v>0.333158965146682</v>
       </c>
       <c r="F84" t="n">
-        <v>0.007078714686950594</v>
+        <v>0.00471914312463373</v>
       </c>
       <c r="G84" t="n">
-        <v>0.008067414723100965</v>
+        <v>0.005378276482067309</v>
       </c>
       <c r="H84" t="n">
-        <v>1.138118878905304</v>
+        <v>0.7587459192702027</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>0.001535312101825481</v>
+        <v>0.001023541401216987</v>
       </c>
       <c r="B85" t="n">
-        <v>0.001443782586458091</v>
+        <v>0.0009625217243053943</v>
       </c>
       <c r="C85" t="n">
-        <v>2.689332984082392</v>
+        <v>1.792888656054928</v>
       </c>
       <c r="D85" t="n">
-        <v>0.2524814382476089</v>
+        <v>0.1683209588317393</v>
       </c>
       <c r="E85" t="n">
-        <v>0.3508471466520536</v>
+        <v>0.2338980977680357</v>
       </c>
       <c r="F85" t="n">
-        <v>0.002600791040331008</v>
+        <v>0.001733860693554006</v>
       </c>
       <c r="G85" t="n">
-        <v>0.009880164624214682</v>
+        <v>0.006586776416143122</v>
       </c>
       <c r="H85" t="n">
-        <v>1.217619976464806</v>
+        <v>0.8117466509765376</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>0.0008151836700620425</v>
+        <v>0.0005434557800413617</v>
       </c>
       <c r="B86" t="n">
-        <v>0.002759707782101291</v>
+        <v>0.001839805188067528</v>
       </c>
       <c r="C86" t="n">
-        <v>2.200123151986451</v>
+        <v>1.466748767990968</v>
       </c>
       <c r="D86" t="n">
-        <v>0.733444372292841</v>
+        <v>0.488962914861894</v>
       </c>
       <c r="E86" t="n">
-        <v>0.4069967182737265</v>
+        <v>0.2713311455158177</v>
       </c>
       <c r="F86" t="n">
-        <v>0.005523625802989999</v>
+        <v>0.003682417201993333</v>
       </c>
       <c r="G86" t="n">
-        <v>0.006885290857220932</v>
+        <v>0.004590193904813955</v>
       </c>
       <c r="H86" t="n">
-        <v>1.172698159801654</v>
+        <v>0.7817987732011029</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>0.001256379263051055</v>
+        <v>0.0008375861753673702</v>
       </c>
       <c r="B87" t="n">
-        <v>0.006616280558859023</v>
+        <v>0.004410853705906016</v>
       </c>
       <c r="C87" t="n">
-        <v>2.056244757867123</v>
+        <v>1.370829838578082</v>
       </c>
       <c r="D87" t="n">
-        <v>0.8254508721372735</v>
+        <v>0.5503005814248491</v>
       </c>
       <c r="E87" t="n">
-        <v>0.4987358638760866</v>
+        <v>0.3324905759173911</v>
       </c>
       <c r="F87" t="n">
-        <v>0.007094279455657515</v>
+        <v>0.00472951963710501</v>
       </c>
       <c r="G87" t="n">
-        <v>0.006737627881780875</v>
+        <v>0.00449175192118725</v>
       </c>
       <c r="H87" t="n">
-        <v>1.148737469249451</v>
+        <v>0.7658249794996342</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>0.0007725923737030229</v>
+        <v>0.0005150615824686819</v>
       </c>
       <c r="B88" t="n">
-        <v>0.001162453329723877</v>
+        <v>0.0007749688864825847</v>
       </c>
       <c r="C88" t="n">
-        <v>2.632871425458627</v>
+        <v>1.755247616972418</v>
       </c>
       <c r="D88" t="n">
-        <v>0.3423698252340088</v>
+        <v>0.2282465501560059</v>
       </c>
       <c r="E88" t="n">
-        <v>0.3317813499673395</v>
+        <v>0.221187566644893</v>
       </c>
       <c r="F88" t="n">
-        <v>0.00229032573356916</v>
+        <v>0.00152688382237944</v>
       </c>
       <c r="G88" t="n">
-        <v>0.007147032845228209</v>
+        <v>0.004764688563485472</v>
       </c>
       <c r="H88" t="n">
-        <v>1.192049324008056</v>
+        <v>0.7946995493387037</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>0.002319158426353578</v>
+        <v>0.001546105617569052</v>
       </c>
       <c r="B89" t="n">
-        <v>0.003198651793728213</v>
+        <v>0.002132434529152142</v>
       </c>
       <c r="C89" t="n">
-        <v>2.644007046036198</v>
+        <v>1.762671364024132</v>
       </c>
       <c r="D89" t="n">
-        <v>0.2811489341819778</v>
+        <v>0.1874326227879852</v>
       </c>
       <c r="E89" t="n">
-        <v>0.3397371098325602</v>
+        <v>0.2264914065550401</v>
       </c>
       <c r="F89" t="n">
-        <v>0.003273843826930987</v>
+        <v>0.002182562551287325</v>
       </c>
       <c r="G89" t="n">
-        <v>0.01243702991222639</v>
+        <v>0.008291353274817595</v>
       </c>
       <c r="H89" t="n">
-        <v>1.244618858252698</v>
+        <v>0.8297459055017986</v>
       </c>
     </row>
     <row r="90">
@@ -2772,22 +2772,22 @@
         <v>1e-07</v>
       </c>
       <c r="C90" t="n">
-        <v>2.581904119325673</v>
+        <v>1.721269412883782</v>
       </c>
       <c r="D90" t="n">
-        <v>0.3293019368279705</v>
+        <v>0.2195346245519804</v>
       </c>
       <c r="E90" t="n">
-        <v>0.3920723701797403</v>
+        <v>0.2613815801198269</v>
       </c>
       <c r="F90" t="n">
-        <v>0.003331253396315606</v>
+        <v>0.002220835597543738</v>
       </c>
       <c r="G90" t="n">
-        <v>0.01297150164562744</v>
+        <v>0.008647667763751626</v>
       </c>
       <c r="H90" t="n">
-        <v>1.22481579054785</v>
+        <v>0.8165438603652333</v>
       </c>
     </row>
     <row r="91">
@@ -2798,22 +2798,22 @@
         <v>1e-07</v>
       </c>
       <c r="C91" t="n">
-        <v>2.374986030315726</v>
+        <v>1.583324020210484</v>
       </c>
       <c r="D91" t="n">
-        <v>0.4795822293271191</v>
+        <v>0.3197214862180794</v>
       </c>
       <c r="E91" t="n">
-        <v>0.457968492348581</v>
+        <v>0.3053123282323874</v>
       </c>
       <c r="F91" t="n">
         <v>1e-07</v>
       </c>
       <c r="G91" t="n">
-        <v>0.009036024415971905</v>
+        <v>0.006024016277314603</v>
       </c>
       <c r="H91" t="n">
-        <v>1.25114309377118</v>
+        <v>0.8340953958474533</v>
       </c>
     </row>
     <row r="92">
@@ -2824,22 +2824,22 @@
         <v>1e-07</v>
       </c>
       <c r="C92" t="n">
-        <v>2.524069790671163</v>
+        <v>1.682713193780775</v>
       </c>
       <c r="D92" t="n">
-        <v>0.3464961021062645</v>
+        <v>0.2309974014041763</v>
       </c>
       <c r="E92" t="n">
-        <v>0.4217684686710905</v>
+        <v>0.2811789791140603</v>
       </c>
       <c r="F92" t="n">
-        <v>0.001655663555991096</v>
+        <v>0.001103775703994064</v>
       </c>
       <c r="G92" t="n">
-        <v>0.01069251162862308</v>
+        <v>0.007128341085748717</v>
       </c>
       <c r="H92" t="n">
-        <v>1.260034516978155</v>
+        <v>0.8400230113187703</v>
       </c>
     </row>
     <row r="93">
@@ -2850,22 +2850,22 @@
         <v>1e-07</v>
       </c>
       <c r="C93" t="n">
-        <v>2.571514030318522</v>
+        <v>1.714342686879015</v>
       </c>
       <c r="D93" t="n">
-        <v>0.3342017377986539</v>
+        <v>0.2228011585324359</v>
       </c>
       <c r="E93" t="n">
-        <v>0.4008186499682418</v>
+        <v>0.2672124333121612</v>
       </c>
       <c r="F93" t="n">
-        <v>0.002994665270925752</v>
+        <v>0.001996443513950502</v>
       </c>
       <c r="G93" t="n">
-        <v>0.01011240568729229</v>
+        <v>0.006741603791528195</v>
       </c>
       <c r="H93" t="n">
-        <v>1.227500626897776</v>
+        <v>0.8183337512651836</v>
       </c>
     </row>
     <row r="94">
@@ -2876,22 +2876,22 @@
         <v>1e-07</v>
       </c>
       <c r="C94" t="n">
-        <v>2.371652167750542</v>
+        <v>1.581101445167028</v>
       </c>
       <c r="D94" t="n">
-        <v>0.4943164718023277</v>
+        <v>0.3295443145348851</v>
       </c>
       <c r="E94" t="n">
-        <v>0.6025166339292959</v>
+        <v>0.4016777559528639</v>
       </c>
       <c r="F94" t="n">
         <v>1e-07</v>
       </c>
       <c r="G94" t="n">
-        <v>0.005995269545741363</v>
+        <v>0.003996846363827575</v>
       </c>
       <c r="H94" t="n">
-        <v>1.09253513719566</v>
+        <v>0.7283567581304395</v>
       </c>
     </row>
     <row r="95">
@@ -2899,25 +2899,25 @@
         <v>1e-07</v>
       </c>
       <c r="B95" t="n">
-        <v>0.003671832052991588</v>
+        <v>0.002447888035327725</v>
       </c>
       <c r="C95" t="n">
-        <v>2.459120736863916</v>
+        <v>1.639413824575944</v>
       </c>
       <c r="D95" t="n">
-        <v>0.4244727626385993</v>
+        <v>0.2829818417590663</v>
       </c>
       <c r="E95" t="n">
-        <v>0.520425999823257</v>
+        <v>0.346950666548838</v>
       </c>
       <c r="F95" t="n">
-        <v>0.006200943095539135</v>
+        <v>0.004133962063692757</v>
       </c>
       <c r="G95" t="n">
-        <v>0.007197913957839984</v>
+        <v>0.004798609305226656</v>
       </c>
       <c r="H95" t="n">
-        <v>1.127776011596537</v>
+        <v>0.7518506743976915</v>
       </c>
     </row>
     <row r="96">
@@ -2925,25 +2925,25 @@
         <v>1e-07</v>
       </c>
       <c r="B96" t="n">
-        <v>0.003007997674586726</v>
+        <v>0.002005331783057817</v>
       </c>
       <c r="C96" t="n">
-        <v>2.516400006002097</v>
+        <v>1.677600004001399</v>
       </c>
       <c r="D96" t="n">
-        <v>0.3635378802715975</v>
+        <v>0.2423585868477317</v>
       </c>
       <c r="E96" t="n">
-        <v>0.4948860402200405</v>
+        <v>0.3299240268133604</v>
       </c>
       <c r="F96" t="n">
-        <v>0.005418525943434176</v>
+        <v>0.003612350628956118</v>
       </c>
       <c r="G96" t="n">
-        <v>0.006754282145207313</v>
+        <v>0.004502854763471542</v>
       </c>
       <c r="H96" t="n">
-        <v>1.16230592955462</v>
+        <v>0.7748706197030804</v>
       </c>
     </row>
     <row r="97">
@@ -2951,25 +2951,25 @@
         <v>1e-07</v>
       </c>
       <c r="B97" t="n">
-        <v>0.002986473945858088</v>
+        <v>0.001990982630572059</v>
       </c>
       <c r="C97" t="n">
-        <v>2.559216228135192</v>
+        <v>1.706144152090128</v>
       </c>
       <c r="D97" t="n">
-        <v>0.3515208478090794</v>
+        <v>0.2343472318727197</v>
       </c>
       <c r="E97" t="n">
-        <v>0.411667334350239</v>
+        <v>0.274444889566826</v>
       </c>
       <c r="F97" t="n">
-        <v>0.004707284468758739</v>
+        <v>0.00313818964583916</v>
       </c>
       <c r="G97" t="n">
-        <v>0.006386620834519258</v>
+        <v>0.004257747223012839</v>
       </c>
       <c r="H97" t="n">
-        <v>1.201332189416661</v>
+        <v>0.8008881262777741</v>
       </c>
     </row>
     <row r="98">
@@ -2977,129 +2977,129 @@
         <v>1e-07</v>
       </c>
       <c r="B98" t="n">
-        <v>0.002663285793620202</v>
+        <v>0.001775523862413468</v>
       </c>
       <c r="C98" t="n">
-        <v>2.572937107587908</v>
+        <v>1.715291405058605</v>
       </c>
       <c r="D98" t="n">
-        <v>0.3296518082842633</v>
+        <v>0.2197678721895089</v>
       </c>
       <c r="E98" t="n">
-        <v>0.3947503292457313</v>
+        <v>0.2631668861638209</v>
       </c>
       <c r="F98" t="n">
-        <v>0.003664811372504635</v>
+        <v>0.002443207581669756</v>
       </c>
       <c r="G98" t="n">
-        <v>0.006328308844840662</v>
+        <v>0.004218872563227108</v>
       </c>
       <c r="H98" t="n">
-        <v>1.231410645223255</v>
+        <v>0.8209404301488364</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>0.006734657083343118</v>
+        <v>0.004489771388895412</v>
       </c>
       <c r="B99" t="n">
-        <v>0.01621289532239673</v>
+        <v>0.01080859688159782</v>
       </c>
       <c r="C99" t="n">
-        <v>1.727680578825106</v>
+        <v>1.151787052550071</v>
       </c>
       <c r="D99" t="n">
-        <v>1.052135985420109</v>
+        <v>0.701423990280073</v>
       </c>
       <c r="E99" t="n">
-        <v>0.7836240966639377</v>
+        <v>0.5224160644426252</v>
       </c>
       <c r="F99" t="n">
-        <v>0.00950698980641284</v>
+        <v>0.006337993204275227</v>
       </c>
       <c r="G99" t="n">
         <v>1e-07</v>
       </c>
       <c r="H99" t="n">
-        <v>0.9912489623503461</v>
+        <v>0.6608326415668975</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>0.006456406674147524</v>
+        <v>0.004304271116098349</v>
       </c>
       <c r="B100" t="n">
-        <v>0.01230490679998048</v>
+        <v>0.008203271199986987</v>
       </c>
       <c r="C100" t="n">
-        <v>1.938352211244285</v>
+        <v>1.29223480749619</v>
       </c>
       <c r="D100" t="n">
-        <v>0.9038516116566786</v>
+        <v>0.6025677411044522</v>
       </c>
       <c r="E100" t="n">
-        <v>0.5737848021001729</v>
+        <v>0.3825232014001152</v>
       </c>
       <c r="F100" t="n">
-        <v>0.006562221952484132</v>
+        <v>0.004374814634989421</v>
       </c>
       <c r="G100" t="n">
-        <v>0.01004095769638994</v>
+        <v>0.006693971797593295</v>
       </c>
       <c r="H100" t="n">
-        <v>1.108783656951251</v>
+        <v>0.7391891046341672</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>0.00467312805967365</v>
+        <v>0.0031154187064491</v>
       </c>
       <c r="B101" t="n">
-        <v>0.01182529093839805</v>
+        <v>0.007883527292265366</v>
       </c>
       <c r="C101" t="n">
-        <v>2.016288459575356</v>
+        <v>1.344192306383571</v>
       </c>
       <c r="D101" t="n">
-        <v>0.8541434300107038</v>
+        <v>0.5694289533404692</v>
       </c>
       <c r="E101" t="n">
-        <v>0.5069907962577677</v>
+        <v>0.3379938641718452</v>
       </c>
       <c r="F101" t="n">
-        <v>0.005757232539692647</v>
+        <v>0.003838155026461765</v>
       </c>
       <c r="G101" t="n">
-        <v>0.009910384759560213</v>
+        <v>0.006606923173040142</v>
       </c>
       <c r="H101" t="n">
-        <v>1.138696914067746</v>
+        <v>0.7591312760451638</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>0.009345229631471878</v>
+        <v>0.006230153087647918</v>
       </c>
       <c r="B102" t="n">
-        <v>0.01246312689365649</v>
+        <v>0.008308751262437662</v>
       </c>
       <c r="C102" t="n">
-        <v>2.021574025035832</v>
+        <v>1.347716016690555</v>
       </c>
       <c r="D102" t="n">
-        <v>0.8587514272805223</v>
+        <v>0.5725009515203482</v>
       </c>
       <c r="E102" t="n">
-        <v>0.4841994116955101</v>
+        <v>0.3227996077970067</v>
       </c>
       <c r="F102" t="n">
-        <v>0.004317450172414638</v>
+        <v>0.002878300114943092</v>
       </c>
       <c r="G102" t="n">
-        <v>0.0102509961870273</v>
+        <v>0.006833997458018198</v>
       </c>
       <c r="H102" t="n">
-        <v>1.136672121813046</v>
+        <v>0.7577814145420304</v>
       </c>
     </row>
     <row r="103">
@@ -3107,25 +3107,25 @@
         <v>1e-07</v>
       </c>
       <c r="B103" t="n">
-        <v>0.003787114151180894</v>
+        <v>0.00252474276745393</v>
       </c>
       <c r="C103" t="n">
-        <v>2.626006673376392</v>
+        <v>1.750671115584262</v>
       </c>
       <c r="D103" t="n">
-        <v>0.3526889528746661</v>
+        <v>0.2351259685831107</v>
       </c>
       <c r="E103" t="n">
-        <v>0.3183351191100302</v>
+        <v>0.2122234127400201</v>
       </c>
       <c r="F103" t="n">
         <v>1e-07</v>
       </c>
       <c r="G103" t="n">
-        <v>0.005918355546260933</v>
+        <v>0.003945570364173956</v>
       </c>
       <c r="H103" t="n">
-        <v>1.200128857664758</v>
+        <v>0.8000859051098383</v>
       </c>
     </row>
     <row r="104">
@@ -3136,13 +3136,13 @@
         <v>1e-07</v>
       </c>
       <c r="C104" t="n">
-        <v>1.607473063657102</v>
+        <v>1.071648709104735</v>
       </c>
       <c r="D104" t="n">
-        <v>1.320279508444782</v>
+        <v>0.8801863389631879</v>
       </c>
       <c r="E104" t="n">
-        <v>0.5396106781033582</v>
+        <v>0.3597404520689055</v>
       </c>
       <c r="F104" t="n">
         <v>1e-07</v>
@@ -3151,7 +3151,7 @@
         <v>1e-07</v>
       </c>
       <c r="H104" t="n">
-        <v>1.068760463743815</v>
+        <v>0.7125069758292103</v>
       </c>
     </row>
     <row r="105">
@@ -3162,13 +3162,13 @@
         <v>1e-07</v>
       </c>
       <c r="C105" t="n">
-        <v>1.921652060271027</v>
+        <v>1.281101373514018</v>
       </c>
       <c r="D105" t="n">
-        <v>0.9736132277678829</v>
+        <v>0.6490754851785886</v>
       </c>
       <c r="E105" t="n">
-        <v>0.5569137538959514</v>
+        <v>0.3712758359306343</v>
       </c>
       <c r="F105" t="n">
         <v>1e-07</v>
@@ -3177,7 +3177,7 @@
         <v>1e-07</v>
       </c>
       <c r="H105" t="n">
-        <v>1.100188314045683</v>
+        <v>0.7334588760304552</v>
       </c>
     </row>
     <row r="106">
@@ -3185,16 +3185,16 @@
         <v>1e-07</v>
       </c>
       <c r="B106" t="n">
-        <v>0.003539341511526175</v>
+        <v>0.002359561007684117</v>
       </c>
       <c r="C106" t="n">
-        <v>1.070140260200303</v>
+        <v>0.713426840133535</v>
       </c>
       <c r="D106" t="n">
-        <v>1.837484789690185</v>
+        <v>1.224989859793456</v>
       </c>
       <c r="E106" t="n">
-        <v>0.691683367101095</v>
+        <v>0.4611222447340633</v>
       </c>
       <c r="F106" t="n">
         <v>1e-07</v>
@@ -3203,7 +3203,7 @@
         <v>1e-07</v>
       </c>
       <c r="H106" t="n">
-        <v>0.9398003750401221</v>
+        <v>0.6265335833600814</v>
       </c>
     </row>
     <row r="107">
@@ -3211,155 +3211,155 @@
         <v>1e-07</v>
       </c>
       <c r="B107" t="n">
-        <v>0.00142629961756312</v>
+        <v>0.0009508664117087468</v>
       </c>
       <c r="C107" t="n">
-        <v>2.81094489054427</v>
+        <v>1.873963260362847</v>
       </c>
       <c r="D107" t="n">
-        <v>0.1492947164345471</v>
+        <v>0.09952981095636471</v>
       </c>
       <c r="E107" t="n">
-        <v>0.3031549371487799</v>
+        <v>0.20210329143252</v>
       </c>
       <c r="F107" t="n">
-        <v>0.003211622114176765</v>
+        <v>0.002141081409451176</v>
       </c>
       <c r="G107" t="n">
-        <v>0.01494580284067169</v>
+        <v>0.009963868560447795</v>
       </c>
       <c r="H107" t="n">
-        <v>1.232834481661949</v>
+        <v>0.8218896544412992</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>0.006228349895085816</v>
+        <v>0.004152233263390544</v>
       </c>
       <c r="B108" t="n">
-        <v>0.00322137154433329</v>
+        <v>0.002147581029555527</v>
       </c>
       <c r="C108" t="n">
-        <v>2.609109376252967</v>
+        <v>1.739406250835311</v>
       </c>
       <c r="D108" t="n">
-        <v>0.3530090869389955</v>
+        <v>0.2353393912926637</v>
       </c>
       <c r="E108" t="n">
-        <v>0.3454057067204411</v>
+        <v>0.2302704711469608</v>
       </c>
       <c r="F108" t="n">
-        <v>0.006594195320256725</v>
+        <v>0.004396130213504484</v>
       </c>
       <c r="G108" t="n">
-        <v>0.009394026805408571</v>
+        <v>0.006262684536939048</v>
       </c>
       <c r="H108" t="n">
-        <v>1.176278685203447</v>
+        <v>0.7841857901356316</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>0.006637552165562817</v>
+        <v>0.004425034777041878</v>
       </c>
       <c r="B109" t="n">
-        <v>0.002349871565699534</v>
+        <v>0.00156658104379969</v>
       </c>
       <c r="C109" t="n">
-        <v>2.575552283398078</v>
+        <v>1.717034855598719</v>
       </c>
       <c r="D109" t="n">
-        <v>0.385250364760036</v>
+        <v>0.2568335765066906</v>
       </c>
       <c r="E109" t="n">
-        <v>0.3392950125533133</v>
+        <v>0.2261966750355422</v>
       </c>
       <c r="F109" t="n">
-        <v>0.0105824882695684</v>
+        <v>0.007054992179712264</v>
       </c>
       <c r="G109" t="n">
-        <v>0.008794164356036478</v>
+        <v>0.005862776237357652</v>
       </c>
       <c r="H109" t="n">
-        <v>1.182149515121387</v>
+        <v>0.7880996767475911</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>0.004350042610224382</v>
+        <v>0.002900028406816255</v>
       </c>
       <c r="B110" t="n">
-        <v>0.007735159745596719</v>
+        <v>0.005156773163731145</v>
       </c>
       <c r="C110" t="n">
-        <v>2.487914395146883</v>
+        <v>1.658609596764588</v>
       </c>
       <c r="D110" t="n">
-        <v>0.4524168841013153</v>
+        <v>0.3016112560675435</v>
       </c>
       <c r="E110" t="n">
-        <v>0.3892587590621616</v>
+        <v>0.2595058393747744</v>
       </c>
       <c r="F110" t="n">
-        <v>0.003349497187006032</v>
+        <v>0.002232998124670688</v>
       </c>
       <c r="G110" t="n">
-        <v>0.01113387627645885</v>
+        <v>0.007422584184305897</v>
       </c>
       <c r="H110" t="n">
-        <v>1.153116364388868</v>
+        <v>0.7687442429259118</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>0.01591973700426909</v>
+        <v>0.01061315800284606</v>
       </c>
       <c r="B111" t="n">
-        <v>0.003213215332184798</v>
+        <v>0.002142143554789866</v>
       </c>
       <c r="C111" t="n">
-        <v>2.632248865254053</v>
+        <v>1.754832576836035</v>
       </c>
       <c r="D111" t="n">
-        <v>0.3033041998791535</v>
+        <v>0.2022027999194357</v>
       </c>
       <c r="E111" t="n">
-        <v>0.3614167710696371</v>
+        <v>0.2409445140464247</v>
       </c>
       <c r="F111" t="n">
-        <v>0.006577499433042096</v>
+        <v>0.004384999622028063</v>
       </c>
       <c r="G111" t="n">
-        <v>0.01155663180757187</v>
+        <v>0.007704421205047913</v>
       </c>
       <c r="H111" t="n">
-        <v>1.176773472997358</v>
+        <v>0.7845156486649053</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>0.00274594494890287</v>
+        <v>0.001830629965935247</v>
       </c>
       <c r="B112" t="n">
-        <v>0.001475566897397672</v>
+        <v>0.0009837112649317816</v>
       </c>
       <c r="C112" t="n">
-        <v>2.527545007208999</v>
+        <v>1.685030004806</v>
       </c>
       <c r="D112" t="n">
-        <v>0.4462970615639211</v>
+        <v>0.2975313743759475</v>
       </c>
       <c r="E112" t="n">
-        <v>0.3447923387449446</v>
+        <v>0.2298615591632964</v>
       </c>
       <c r="F112" t="n">
-        <v>0.001993534831086712</v>
+        <v>0.001329023220724475</v>
       </c>
       <c r="G112" t="n">
-        <v>0.002839970418106318</v>
+        <v>0.001893313612070879</v>
       </c>
       <c r="H112" t="n">
-        <v>1.157877022211775</v>
+        <v>0.7719180148078498</v>
       </c>
     </row>
     <row r="113">
@@ -3367,415 +3367,415 @@
         <v>1e-07</v>
       </c>
       <c r="B113" t="n">
-        <v>0.003786800544173973</v>
+        <v>0.002524533696115982</v>
       </c>
       <c r="C113" t="n">
-        <v>2.659102148839718</v>
+        <v>1.772734765893145</v>
       </c>
       <c r="D113" t="n">
-        <v>0.2801073511861594</v>
+        <v>0.1867382341241063</v>
       </c>
       <c r="E113" t="n">
-        <v>0.3461567267725645</v>
+        <v>0.2307711511817097</v>
       </c>
       <c r="F113" t="n">
-        <v>0.00327953867473364</v>
+        <v>0.002186359116489093</v>
       </c>
       <c r="G113" t="n">
-        <v>0.01401599712637379</v>
+        <v>0.009343998084249192</v>
       </c>
       <c r="H113" t="n">
-        <v>1.215614274627669</v>
+        <v>0.8104095164184463</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>0.02770948997918783</v>
+        <v>0.01847299331945855</v>
       </c>
       <c r="B114" t="n">
-        <v>0.002978006254160222</v>
+        <v>0.001985337502773481</v>
       </c>
       <c r="C114" t="n">
-        <v>2.44932171718957</v>
+        <v>1.632881144793046</v>
       </c>
       <c r="D114" t="n">
-        <v>0.497619125708735</v>
+        <v>0.3317460838058233</v>
       </c>
       <c r="E114" t="n">
-        <v>0.3442904185012616</v>
+        <v>0.2295269456675077</v>
       </c>
       <c r="F114" t="n">
-        <v>0.0100584378880629</v>
+        <v>0.006705625258708602</v>
       </c>
       <c r="G114" t="n">
-        <v>0.01910553763362926</v>
+        <v>0.01273702508908617</v>
       </c>
       <c r="H114" t="n">
-        <v>1.138914862328346</v>
+        <v>0.7592765748855641</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>0.07188787257869036</v>
+        <v>0.04792524838579357</v>
       </c>
       <c r="B115" t="n">
-        <v>0.003004541725373689</v>
+        <v>0.002003027816915792</v>
       </c>
       <c r="C115" t="n">
-        <v>2.226385191621468</v>
+        <v>1.484256794414312</v>
       </c>
       <c r="D115" t="n">
-        <v>0.6094104297694588</v>
+        <v>0.4062736198463059</v>
       </c>
       <c r="E115" t="n">
-        <v>0.3473582120884812</v>
+        <v>0.2315721413923208</v>
       </c>
       <c r="F115" t="n">
-        <v>0.006765375612077467</v>
+        <v>0.004510250408051645</v>
       </c>
       <c r="G115" t="n">
-        <v>0.009637888591695348</v>
+        <v>0.006425259061130231</v>
       </c>
       <c r="H115" t="n">
-        <v>1.196692703063986</v>
+        <v>0.7977951353759907</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>0.003871469147621298</v>
+        <v>0.002580979431747532</v>
       </c>
       <c r="B116" t="n">
         <v>1e-07</v>
       </c>
       <c r="C116" t="n">
-        <v>2.619049656768083</v>
+        <v>1.746033104512055</v>
       </c>
       <c r="D116" t="n">
-        <v>0.327513365378136</v>
+        <v>0.218342243585424</v>
       </c>
       <c r="E116" t="n">
-        <v>0.3270079277385666</v>
+        <v>0.2180052851590444</v>
       </c>
       <c r="F116" t="n">
-        <v>0.006558198987736455</v>
+        <v>0.004372132658490969</v>
       </c>
       <c r="G116" t="n">
-        <v>0.01245699570484285</v>
+        <v>0.008304663803228564</v>
       </c>
       <c r="H116" t="n">
-        <v>1.22353140950934</v>
+        <v>0.8156876063395599</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>0.0353902499477036</v>
+        <v>0.02359349996513573</v>
       </c>
       <c r="B117" t="n">
-        <v>0.002958259267524887</v>
+        <v>0.001972172845016591</v>
       </c>
       <c r="C117" t="n">
-        <v>2.456252601388083</v>
+        <v>1.637501734258722</v>
       </c>
       <c r="D117" t="n">
-        <v>0.4849926602390502</v>
+        <v>0.3233284401593668</v>
       </c>
       <c r="E117" t="n">
-        <v>0.3452959818786799</v>
+        <v>0.2301973212524533</v>
       </c>
       <c r="F117" t="n">
-        <v>0.009991740970193624</v>
+        <v>0.006661160646795749</v>
       </c>
       <c r="G117" t="n">
-        <v>0.01897884992241807</v>
+        <v>0.01265256661494538</v>
       </c>
       <c r="H117" t="n">
-        <v>1.131362783976005</v>
+        <v>0.754241855984003</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>0.003891531622514007</v>
+        <v>0.002594354415009338</v>
       </c>
       <c r="B118" t="n">
-        <v>0.002927626550748251</v>
+        <v>0.001951751033832167</v>
       </c>
       <c r="C118" t="n">
-        <v>2.577584532905111</v>
+        <v>1.718389688603407</v>
       </c>
       <c r="D118" t="n">
-        <v>0.3507477247722932</v>
+        <v>0.2338318165148621</v>
       </c>
       <c r="E118" t="n">
-        <v>0.3482294096776274</v>
+        <v>0.232152939785085</v>
       </c>
       <c r="F118" t="n">
-        <v>0.003296092229379718</v>
+        <v>0.002197394819586479</v>
       </c>
       <c r="G118" t="n">
-        <v>0.01252154953545274</v>
+        <v>0.00834769969030183</v>
       </c>
       <c r="H118" t="n">
-        <v>1.224070631558466</v>
+        <v>0.8160470877056439</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>0.00785980232418293</v>
+        <v>0.005239868216121954</v>
       </c>
       <c r="B119" t="n">
-        <v>0.005912984449306742</v>
+        <v>0.003941989632871163</v>
       </c>
       <c r="C119" t="n">
-        <v>2.496470455189369</v>
+        <v>1.664313636792913</v>
       </c>
       <c r="D119" t="n">
-        <v>0.4474181186685822</v>
+        <v>0.2982787457790548</v>
       </c>
       <c r="E119" t="n">
-        <v>0.3220837460212442</v>
+        <v>0.2147224973474962</v>
       </c>
       <c r="F119" t="n">
-        <v>0.003328590883769281</v>
+        <v>0.002219060589179521</v>
       </c>
       <c r="G119" t="n">
-        <v>0.01264500891779262</v>
+        <v>0.008430005945195078</v>
       </c>
       <c r="H119" t="n">
-        <v>1.218564219843287</v>
+        <v>0.8123761465621911</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>0.02130105887260235</v>
+        <v>0.01420070591506823</v>
       </c>
       <c r="B120" t="n">
-        <v>0.003204987216534319</v>
+        <v>0.002136658144356213</v>
       </c>
       <c r="C120" t="n">
-        <v>2.038511939969918</v>
+        <v>1.359007959979945</v>
       </c>
       <c r="D120" t="n">
-        <v>0.9060515667456209</v>
+        <v>0.6040343778304139</v>
       </c>
       <c r="E120" t="n">
-        <v>0.5130442038720829</v>
+        <v>0.3420294692480553</v>
       </c>
       <c r="F120" t="n">
-        <v>0.007216721994121921</v>
+        <v>0.004811147996081282</v>
       </c>
       <c r="G120" t="n">
-        <v>0.01370782970323533</v>
+        <v>0.009138553135490224</v>
       </c>
       <c r="H120" t="n">
-        <v>0.9907389696200893</v>
+        <v>0.6604926464133929</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>0.007698413268714539</v>
+        <v>0.005132275512476359</v>
       </c>
       <c r="B121" t="n">
-        <v>0.002895785165117233</v>
+        <v>0.001930523443411489</v>
       </c>
       <c r="C121" t="n">
-        <v>2.649354725171084</v>
+        <v>1.766236483447389</v>
       </c>
       <c r="D121" t="n">
-        <v>0.2921540465739024</v>
+        <v>0.1947693643826016</v>
       </c>
       <c r="E121" t="n">
-        <v>0.3315656682234431</v>
+        <v>0.2210437788156287</v>
       </c>
       <c r="F121" t="n">
-        <v>0.003260243345674159</v>
+        <v>0.002173495563782772</v>
       </c>
       <c r="G121" t="n">
-        <v>0.01238536294179231</v>
+        <v>0.008256908627861541</v>
       </c>
       <c r="H121" t="n">
-        <v>1.216495609094943</v>
+        <v>0.8109970727299624</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>0.06186936225358033</v>
+        <v>0.04124624150238689</v>
       </c>
       <c r="B122" t="n">
-        <v>0.002909047214269288</v>
+        <v>0.001939364809512859</v>
       </c>
       <c r="C122" t="n">
-        <v>2.529325237615655</v>
+        <v>1.686216825077103</v>
       </c>
       <c r="D122" t="n">
-        <v>0.3546362232667303</v>
+        <v>0.2364241488444868</v>
       </c>
       <c r="E122" t="n">
-        <v>0.2748752817249516</v>
+        <v>0.1832501878166344</v>
       </c>
       <c r="F122" t="n">
-        <v>0.006550349063749995</v>
+        <v>0.004366899375833329</v>
       </c>
       <c r="G122" t="n">
-        <v>0.009331563852927357</v>
+        <v>0.006221042568618237</v>
       </c>
       <c r="H122" t="n">
-        <v>1.250889219471338</v>
+        <v>0.8339261463142253</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>0.02767994957881479</v>
+        <v>0.01845329971920986</v>
       </c>
       <c r="B123" t="n">
-        <v>0.008924494426544412</v>
+        <v>0.005949662951029608</v>
       </c>
       <c r="C123" t="n">
-        <v>2.414087748609749</v>
+        <v>1.6093918324065</v>
       </c>
       <c r="D123" t="n">
-        <v>0.5064676569791543</v>
+        <v>0.3376451046527696</v>
       </c>
       <c r="E123" t="n">
-        <v>0.3207746900482018</v>
+        <v>0.2138497933654679</v>
       </c>
       <c r="F123" t="n">
-        <v>0.003349238278923408</v>
+        <v>0.002232825519282272</v>
       </c>
       <c r="G123" t="n">
-        <v>0.02226603130916201</v>
+        <v>0.01484402087277467</v>
       </c>
       <c r="H123" t="n">
-        <v>1.196648915883633</v>
+        <v>0.7977659439224218</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>0.003890448742779582</v>
+        <v>0.002593632495186387</v>
       </c>
       <c r="B124" t="n">
-        <v>0.002926811892724292</v>
+        <v>0.001951207928482862</v>
       </c>
       <c r="C124" t="n">
-        <v>2.567696933374363</v>
+        <v>1.711797955582908</v>
       </c>
       <c r="D124" t="n">
-        <v>0.4213953241129595</v>
+        <v>0.2809302160753063</v>
       </c>
       <c r="E124" t="n">
-        <v>0.3123431859862043</v>
+        <v>0.2082287906574695</v>
       </c>
       <c r="F124" t="n">
-        <v>0.006590350079998466</v>
+        <v>0.004393566719998977</v>
       </c>
       <c r="G124" t="n">
-        <v>0.009388548913367921</v>
+        <v>0.006259032608911947</v>
       </c>
       <c r="H124" t="n">
-        <v>1.17153299985386</v>
+        <v>0.7810219999025731</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>0.01638052073799272</v>
+        <v>0.01092034715866181</v>
       </c>
       <c r="B125" t="n">
-        <v>0.01232318071121037</v>
+        <v>0.008215453807473582</v>
       </c>
       <c r="C125" t="n">
-        <v>2.239451857905525</v>
+        <v>1.49296790527035</v>
       </c>
       <c r="D125" t="n">
-        <v>0.6637293476424851</v>
+        <v>0.4424862317616568</v>
       </c>
       <c r="E125" t="n">
-        <v>0.407545196789562</v>
+        <v>0.271696797859708</v>
       </c>
       <c r="F125" t="n">
-        <v>0.00346853837736589</v>
+        <v>0.002312358918243927</v>
       </c>
       <c r="G125" t="n">
-        <v>0.0230591488797519</v>
+        <v>0.0153727659198346</v>
       </c>
       <c r="H125" t="n">
-        <v>1.147701689473461</v>
+        <v>0.765134459648974</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>0.03155414653887353</v>
+        <v>0.02103609769258235</v>
       </c>
       <c r="B126" t="n">
-        <v>0.002967300736391314</v>
+        <v>0.001978200490927542</v>
       </c>
       <c r="C126" t="n">
-        <v>2.514894399939852</v>
+        <v>1.676596266626568</v>
       </c>
       <c r="D126" t="n">
-        <v>0.4303432395376131</v>
+        <v>0.2868954930250753</v>
       </c>
       <c r="E126" t="n">
-        <v>0.3496499105152912</v>
+        <v>0.2330999403435274</v>
       </c>
       <c r="F126" t="n">
-        <v>0.006681519469723621</v>
+        <v>0.004454346313149081</v>
       </c>
       <c r="G126" t="n">
-        <v>0.01903685588645844</v>
+        <v>0.01269123725763896</v>
       </c>
       <c r="H126" t="n">
-        <v>1.13482062200266</v>
+        <v>0.7565470813351066</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>0.02385217516690364</v>
+        <v>0.01590145011126909</v>
       </c>
       <c r="B127" t="n">
-        <v>0.01196277251656397</v>
+        <v>0.00797518167770931</v>
       </c>
       <c r="C127" t="n">
-        <v>2.46912679531795</v>
+        <v>1.646084530211967</v>
       </c>
       <c r="D127" t="n">
-        <v>0.4274497775392028</v>
+        <v>0.2849665183594685</v>
       </c>
       <c r="E127" t="n">
-        <v>0.3956259827445937</v>
+        <v>0.2637506551630625</v>
       </c>
       <c r="F127" t="n">
-        <v>0.006734192502046753</v>
+        <v>0.004489461668031169</v>
       </c>
       <c r="G127" t="n">
-        <v>0.02558257449353026</v>
+        <v>0.01705504966235351</v>
       </c>
       <c r="H127" t="n">
-        <v>1.14969311014331</v>
+        <v>0.7664620734288734</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>0.003893346307462031</v>
+        <v>0.002595564204974687</v>
       </c>
       <c r="B128" t="n">
         <v>1e-07</v>
       </c>
       <c r="C128" t="n">
-        <v>2.597140855132798</v>
+        <v>1.731427236755199</v>
       </c>
       <c r="D128" t="n">
-        <v>0.3755366374583874</v>
+        <v>0.2503577583055916</v>
       </c>
       <c r="E128" t="n">
-        <v>0.3255998081833433</v>
+        <v>0.2170665387888956</v>
       </c>
       <c r="F128" t="n">
-        <v>0.003297629251184025</v>
+        <v>0.00219841950078935</v>
       </c>
       <c r="G128" t="n">
         <v>1e-07</v>
       </c>
       <c r="H128" t="n">
-        <v>1.201425484358548</v>
+        <v>0.8009503229056988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>